<commit_message>
wk 15 hi score, league history, semifinals vid
</commit_message>
<xml_diff>
--- a/TeamFriends_History.xlsx
+++ b/TeamFriends_History.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Sites\TeamFriendsFantasy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85183C78-4C9A-4FA6-B6FB-15E7E2A346AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{652D32BD-FED8-4607-A692-C54939B1DBD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="677" activeTab="18" xr2:uid="{960D14EB-F112-4860-840A-1E6B67EAFFB3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="677" activeTab="17" xr2:uid="{960D14EB-F112-4860-840A-1E6B67EAFFB3}"/>
   </bookViews>
   <sheets>
     <sheet name="2005" sheetId="16" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1466" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1468" uniqueCount="277">
   <si>
     <t>Team</t>
   </si>
@@ -1124,7 +1124,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1162,6 +1162,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="5" applyBorder="1"/>
     <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="5" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="5" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1174,22 +1175,22 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1198,25 +1199,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="5" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Calculation" xfId="4" builtinId="22"/>
@@ -1663,7 +1645,7 @@
       <c r="I2" s="1">
         <v>2368.5</v>
       </c>
-      <c r="K2" s="39" t="s">
+      <c r="K2" s="40" t="s">
         <v>170</v>
       </c>
     </row>
@@ -1696,8 +1678,8 @@
       <c r="I3" s="1">
         <v>2248.5</v>
       </c>
-      <c r="K3" s="39"/>
-      <c r="L3" s="38" t="s">
+      <c r="K3" s="40"/>
+      <c r="L3" s="39" t="s">
         <v>167</v>
       </c>
     </row>
@@ -1730,10 +1712,10 @@
       <c r="I4" s="1">
         <v>2325.5</v>
       </c>
-      <c r="K4" s="38" t="s">
+      <c r="K4" s="39" t="s">
         <v>167</v>
       </c>
-      <c r="L4" s="38"/>
+      <c r="L4" s="39"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -1764,7 +1746,7 @@
       <c r="I5" s="1">
         <v>2430.5</v>
       </c>
-      <c r="K5" s="38"/>
+      <c r="K5" s="39"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6">
@@ -1822,24 +1804,24 @@
       <c r="I7">
         <v>1856</v>
       </c>
-      <c r="K7" s="37" t="s">
+      <c r="K7" s="38" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K8" s="37"/>
-      <c r="L8" s="37" t="s">
+      <c r="K8" s="38"/>
+      <c r="L8" s="38" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K9" s="38" t="s">
+      <c r="K9" s="39" t="s">
         <v>169</v>
       </c>
-      <c r="L9" s="37"/>
+      <c r="L9" s="38"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K10" s="38"/>
+      <c r="K10" s="39"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L12" s="6" t="s">
@@ -1847,7 +1829,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L13" s="37" t="s">
+      <c r="L13" s="38" t="s">
         <v>170</v>
       </c>
     </row>
@@ -1864,7 +1846,7 @@
       <c r="D14" t="s">
         <v>181</v>
       </c>
-      <c r="L14" s="37"/>
+      <c r="L14" s="38"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1879,7 +1861,7 @@
       <c r="D15">
         <v>0</v>
       </c>
-      <c r="L15" s="38" t="s">
+      <c r="L15" s="39" t="s">
         <v>165</v>
       </c>
     </row>
@@ -1890,7 +1872,7 @@
       <c r="B16" t="s">
         <v>183</v>
       </c>
-      <c r="L16" s="38"/>
+      <c r="L16" s="39"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -2325,7 +2307,7 @@
       <c r="J3" s="1">
         <v>1670.76</v>
       </c>
-      <c r="L3" s="38" t="s">
+      <c r="L3" s="39" t="s">
         <v>97</v>
       </c>
     </row>
@@ -2361,7 +2343,7 @@
       <c r="J4" s="1">
         <v>1595.7</v>
       </c>
-      <c r="L4" s="45"/>
+      <c r="L4" s="42"/>
       <c r="M4" s="10"/>
     </row>
     <row r="5" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2396,7 +2378,7 @@
       <c r="J5" s="1">
         <v>1645.12</v>
       </c>
-      <c r="L5" s="39" t="s">
+      <c r="L5" s="40" t="s">
         <v>80</v>
       </c>
       <c r="N5" s="14"/>
@@ -2433,8 +2415,8 @@
       <c r="J6" s="1">
         <v>1622.42</v>
       </c>
-      <c r="L6" s="39"/>
-      <c r="N6" s="41" t="s">
+      <c r="L6" s="40"/>
+      <c r="N6" s="44" t="s">
         <v>97</v>
       </c>
     </row>
@@ -2467,7 +2449,7 @@
       <c r="J7">
         <v>1329.76</v>
       </c>
-      <c r="N7" s="46"/>
+      <c r="N7" s="45"/>
       <c r="O7" s="10"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -2500,7 +2482,7 @@
       <c r="J8" s="10">
         <v>1426.34</v>
       </c>
-      <c r="N8" s="42" t="s">
+      <c r="N8" s="43" t="s">
         <v>96</v>
       </c>
       <c r="P8" s="14"/>
@@ -2509,10 +2491,10 @@
       <c r="A9" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="L9" s="38" t="s">
+      <c r="L9" s="39" t="s">
         <v>96</v>
       </c>
-      <c r="N9" s="42"/>
+      <c r="N9" s="43"/>
       <c r="P9" s="14"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -2546,7 +2528,7 @@
       <c r="J10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="L10" s="45"/>
+      <c r="L10" s="42"/>
       <c r="M10" s="10"/>
       <c r="N10" s="14"/>
       <c r="P10" s="14"/>
@@ -2583,7 +2565,7 @@
       <c r="J11" s="1">
         <v>1668.7</v>
       </c>
-      <c r="L11" s="37" t="s">
+      <c r="L11" s="38" t="s">
         <v>88</v>
       </c>
       <c r="P11" s="14"/>
@@ -2620,8 +2602,8 @@
       <c r="J12" s="1">
         <v>1621.08</v>
       </c>
-      <c r="L12" s="37"/>
-      <c r="P12" s="42" t="s">
+      <c r="L12" s="38"/>
+      <c r="P12" s="43" t="s">
         <v>96</v>
       </c>
     </row>
@@ -2654,7 +2636,7 @@
       <c r="J13">
         <v>1604.78</v>
       </c>
-      <c r="P13" s="43"/>
+      <c r="P13" s="47"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B14">
@@ -2685,7 +2667,7 @@
       <c r="J14">
         <v>1563.12</v>
       </c>
-      <c r="P14" s="41" t="s">
+      <c r="P14" s="44" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2718,10 +2700,10 @@
       <c r="J15">
         <v>1437.26</v>
       </c>
-      <c r="L15" s="38" t="s">
+      <c r="L15" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="P15" s="41"/>
+      <c r="P15" s="44"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B16">
@@ -2752,12 +2734,12 @@
       <c r="J16">
         <v>1463.6</v>
       </c>
-      <c r="L16" s="45"/>
+      <c r="L16" s="42"/>
       <c r="M16" s="10"/>
       <c r="P16" s="14"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L17" s="37" t="s">
+      <c r="L17" s="38" t="s">
         <v>60</v>
       </c>
       <c r="N17" s="14"/>
@@ -2765,20 +2747,20 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H18" s="4"/>
-      <c r="L18" s="37"/>
-      <c r="N18" s="41" t="s">
+      <c r="L18" s="38"/>
+      <c r="N18" s="44" t="s">
         <v>73</v>
       </c>
       <c r="P18" s="14"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H19" s="4"/>
-      <c r="N19" s="46"/>
+      <c r="N19" s="45"/>
       <c r="O19" s="10"/>
       <c r="P19" s="14"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="N20" s="42" t="s">
+      <c r="N20" s="43" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2792,10 +2774,10 @@
       <c r="F21" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="L21" s="38" t="s">
+      <c r="L21" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="N21" s="42"/>
+      <c r="N21" s="43"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -2810,7 +2792,7 @@
       <c r="F22" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="L22" s="45"/>
+      <c r="L22" s="42"/>
       <c r="M22" s="10"/>
       <c r="N22" s="14"/>
     </row>
@@ -2824,7 +2806,7 @@
       <c r="F23" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="L23" s="37" t="s">
+      <c r="L23" s="38" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2838,7 +2820,7 @@
       <c r="F24" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="L24" s="37"/>
+      <c r="L24" s="38"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -2853,7 +2835,7 @@
       <c r="A26" t="s">
         <v>30</v>
       </c>
-      <c r="P26" s="37" t="s">
+      <c r="P26" s="38" t="s">
         <v>97</v>
       </c>
     </row>
@@ -2861,13 +2843,13 @@
       <c r="A27" t="s">
         <v>83</v>
       </c>
-      <c r="P27" s="44"/>
+      <c r="P27" s="46"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>32</v>
       </c>
-      <c r="P28" s="38" t="s">
+      <c r="P28" s="39" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2875,18 +2857,13 @@
       <c r="A29" t="s">
         <v>49</v>
       </c>
-      <c r="P29" s="38"/>
+      <c r="P29" s="39"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C3:J8">
     <sortCondition descending="1" ref="H3:H8"/>
   </sortState>
   <mergeCells count="16">
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="L9:L10"/>
     <mergeCell ref="L23:L24"/>
     <mergeCell ref="P26:P27"/>
     <mergeCell ref="P28:P29"/>
@@ -2898,6 +2875,11 @@
     <mergeCell ref="N20:N21"/>
     <mergeCell ref="L21:L22"/>
     <mergeCell ref="L11:L12"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="L9:L10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3003,7 +2985,7 @@
       <c r="J3" s="1">
         <v>1593.46</v>
       </c>
-      <c r="L3" s="38" t="s">
+      <c r="L3" s="39" t="s">
         <v>96</v>
       </c>
     </row>
@@ -3039,7 +3021,7 @@
       <c r="J4" s="1">
         <v>1541.96</v>
       </c>
-      <c r="L4" s="45"/>
+      <c r="L4" s="42"/>
       <c r="M4" s="10"/>
     </row>
     <row r="5" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3074,7 +3056,7 @@
       <c r="J5" s="1">
         <v>1469.7</v>
       </c>
-      <c r="L5" s="39" t="s">
+      <c r="L5" s="40" t="s">
         <v>80</v>
       </c>
       <c r="N5" s="14"/>
@@ -3108,8 +3090,8 @@
       <c r="J6">
         <v>1471.44</v>
       </c>
-      <c r="L6" s="39"/>
-      <c r="N6" s="42" t="s">
+      <c r="L6" s="40"/>
+      <c r="N6" s="43" t="s">
         <v>96</v>
       </c>
     </row>
@@ -3142,7 +3124,7 @@
       <c r="J7">
         <v>1396.52</v>
       </c>
-      <c r="N7" s="43"/>
+      <c r="N7" s="47"/>
       <c r="O7" s="10"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -3175,7 +3157,7 @@
       <c r="J8" s="10">
         <v>1071.8599999999999</v>
       </c>
-      <c r="N8" s="41" t="s">
+      <c r="N8" s="44" t="s">
         <v>60</v>
       </c>
       <c r="P8" s="14"/>
@@ -3184,10 +3166,10 @@
       <c r="A9" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="L9" s="37" t="s">
+      <c r="L9" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="N9" s="41"/>
+      <c r="N9" s="44"/>
       <c r="P9" s="14"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -3221,7 +3203,7 @@
       <c r="J10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="L10" s="44"/>
+      <c r="L10" s="46"/>
       <c r="M10" s="10"/>
       <c r="N10" s="14"/>
       <c r="P10" s="14"/>
@@ -3258,7 +3240,7 @@
       <c r="J11" s="1">
         <v>1662.04</v>
       </c>
-      <c r="L11" s="38" t="s">
+      <c r="L11" s="39" t="s">
         <v>60</v>
       </c>
       <c r="P11" s="14"/>
@@ -3295,8 +3277,8 @@
       <c r="J12" s="1">
         <v>1508.68</v>
       </c>
-      <c r="L12" s="38"/>
-      <c r="P12" s="42" t="s">
+      <c r="L12" s="39"/>
+      <c r="P12" s="43" t="s">
         <v>96</v>
       </c>
     </row>
@@ -3332,7 +3314,7 @@
       <c r="J13" s="1">
         <v>1559.22</v>
       </c>
-      <c r="P13" s="43"/>
+      <c r="P13" s="47"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B14">
@@ -3363,7 +3345,7 @@
       <c r="J14">
         <v>1534.62</v>
       </c>
-      <c r="P14" s="41" t="s">
+      <c r="P14" s="44" t="s">
         <v>115</v>
       </c>
     </row>
@@ -3396,10 +3378,10 @@
       <c r="J15">
         <v>1411.74</v>
       </c>
-      <c r="L15" s="38" t="s">
+      <c r="L15" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="P15" s="41"/>
+      <c r="P15" s="44"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B16">
@@ -3430,12 +3412,12 @@
       <c r="J16">
         <v>1163.0999999999999</v>
       </c>
-      <c r="L16" s="45"/>
+      <c r="L16" s="42"/>
       <c r="M16" s="10"/>
       <c r="P16" s="14"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L17" s="37" t="s">
+      <c r="L17" s="38" t="s">
         <v>119</v>
       </c>
       <c r="N17" s="14"/>
@@ -3443,20 +3425,20 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H18" s="4"/>
-      <c r="L18" s="37"/>
-      <c r="N18" s="41" t="s">
+      <c r="L18" s="38"/>
+      <c r="N18" s="44" t="s">
         <v>73</v>
       </c>
       <c r="P18" s="14"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H19" s="4"/>
-      <c r="N19" s="46"/>
+      <c r="N19" s="45"/>
       <c r="O19" s="10"/>
       <c r="P19" s="14"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="N20" s="42" t="s">
+      <c r="N20" s="43" t="s">
         <v>115</v>
       </c>
     </row>
@@ -3470,10 +3452,10 @@
       <c r="F21" s="16">
         <v>200</v>
       </c>
-      <c r="L21" s="38" t="s">
+      <c r="L21" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="N21" s="42"/>
+      <c r="N21" s="43"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -3488,7 +3470,7 @@
       <c r="F22" s="16">
         <v>100</v>
       </c>
-      <c r="L22" s="45"/>
+      <c r="L22" s="42"/>
       <c r="M22" s="10"/>
       <c r="N22" s="14"/>
     </row>
@@ -3502,7 +3484,7 @@
       <c r="F23" s="16">
         <v>40</v>
       </c>
-      <c r="L23" s="37" t="s">
+      <c r="L23" s="38" t="s">
         <v>80</v>
       </c>
     </row>
@@ -3516,7 +3498,7 @@
       <c r="F24" s="16">
         <v>50</v>
       </c>
-      <c r="L24" s="37"/>
+      <c r="L24" s="38"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -3543,7 +3525,7 @@
       <c r="F26" s="16">
         <v>10</v>
       </c>
-      <c r="P26" s="37" t="s">
+      <c r="P26" s="38" t="s">
         <v>60</v>
       </c>
     </row>
@@ -3551,13 +3533,13 @@
       <c r="A27" t="s">
         <v>83</v>
       </c>
-      <c r="P27" s="44"/>
+      <c r="P27" s="46"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>32</v>
       </c>
-      <c r="P28" s="38" t="s">
+      <c r="P28" s="39" t="s">
         <v>73</v>
       </c>
     </row>
@@ -3565,18 +3547,13 @@
       <c r="A29" t="s">
         <v>49</v>
       </c>
-      <c r="P29" s="38"/>
+      <c r="P29" s="39"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C11:J16">
     <sortCondition descending="1" ref="H11:H16"/>
   </sortState>
   <mergeCells count="16">
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="L9:L10"/>
     <mergeCell ref="L23:L24"/>
     <mergeCell ref="P26:P27"/>
     <mergeCell ref="P28:P29"/>
@@ -3588,6 +3565,11 @@
     <mergeCell ref="N20:N21"/>
     <mergeCell ref="L21:L22"/>
     <mergeCell ref="L11:L12"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="L9:L10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3693,7 +3675,7 @@
       <c r="J3" s="1">
         <v>1792.26</v>
       </c>
-      <c r="L3" s="38" t="s">
+      <c r="L3" s="39" t="s">
         <v>123</v>
       </c>
     </row>
@@ -3729,7 +3711,7 @@
       <c r="J4" s="1">
         <v>1746.74</v>
       </c>
-      <c r="L4" s="45"/>
+      <c r="L4" s="42"/>
       <c r="M4" s="10"/>
     </row>
     <row r="5" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3761,7 +3743,7 @@
       <c r="J5">
         <v>1623.88</v>
       </c>
-      <c r="L5" s="39" t="s">
+      <c r="L5" s="40" t="s">
         <v>80</v>
       </c>
       <c r="N5" s="14"/>
@@ -3795,8 +3777,8 @@
       <c r="J6">
         <v>1608.62</v>
       </c>
-      <c r="L6" s="39"/>
-      <c r="N6" s="41" t="s">
+      <c r="L6" s="40"/>
+      <c r="N6" s="44" t="s">
         <v>123</v>
       </c>
     </row>
@@ -3829,7 +3811,7 @@
       <c r="J7">
         <v>1608.1</v>
       </c>
-      <c r="N7" s="46"/>
+      <c r="N7" s="45"/>
       <c r="O7" s="10"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -3862,7 +3844,7 @@
       <c r="J8" s="10">
         <v>1419.32</v>
       </c>
-      <c r="N8" s="42" t="s">
+      <c r="N8" s="43" t="s">
         <v>116</v>
       </c>
       <c r="P8" s="14"/>
@@ -3871,10 +3853,10 @@
       <c r="A9" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="L9" s="38" t="s">
+      <c r="L9" s="39" t="s">
         <v>116</v>
       </c>
-      <c r="N9" s="42"/>
+      <c r="N9" s="43"/>
       <c r="P9" s="14"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -3908,7 +3890,7 @@
       <c r="J10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="L10" s="45"/>
+      <c r="L10" s="42"/>
       <c r="M10" s="10"/>
       <c r="N10" s="14"/>
       <c r="P10" s="14"/>
@@ -3945,7 +3927,7 @@
       <c r="J11" s="1">
         <v>1895.72</v>
       </c>
-      <c r="L11" s="37" t="s">
+      <c r="L11" s="38" t="s">
         <v>124</v>
       </c>
       <c r="P11" s="14"/>
@@ -3982,8 +3964,8 @@
       <c r="J12" s="1">
         <v>1666.54</v>
       </c>
-      <c r="L12" s="37"/>
-      <c r="P12" s="41" t="s">
+      <c r="L12" s="38"/>
+      <c r="P12" s="44" t="s">
         <v>116</v>
       </c>
     </row>
@@ -4019,7 +4001,7 @@
       <c r="J13" s="1">
         <v>1770.32</v>
       </c>
-      <c r="P13" s="46"/>
+      <c r="P13" s="45"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -4053,7 +4035,7 @@
       <c r="J14" s="1">
         <v>1642.38</v>
       </c>
-      <c r="P14" s="42" t="s">
+      <c r="P14" s="43" t="s">
         <v>122</v>
       </c>
     </row>
@@ -4086,10 +4068,10 @@
       <c r="J15">
         <v>1496.7</v>
       </c>
-      <c r="L15" s="37" t="s">
+      <c r="L15" s="38" t="s">
         <v>115</v>
       </c>
-      <c r="P15" s="42"/>
+      <c r="P15" s="43"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B16">
@@ -4120,12 +4102,12 @@
       <c r="J16">
         <v>1310.1400000000001</v>
       </c>
-      <c r="L16" s="44"/>
+      <c r="L16" s="46"/>
       <c r="M16" s="10"/>
       <c r="P16" s="14"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L17" s="38" t="s">
+      <c r="L17" s="39" t="s">
         <v>122</v>
       </c>
       <c r="N17" s="14"/>
@@ -4133,20 +4115,20 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H18" s="4"/>
-      <c r="L18" s="38"/>
-      <c r="N18" s="42" t="s">
+      <c r="L18" s="39"/>
+      <c r="N18" s="43" t="s">
         <v>122</v>
       </c>
       <c r="P18" s="14"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H19" s="4"/>
-      <c r="N19" s="43"/>
+      <c r="N19" s="47"/>
       <c r="O19" s="10"/>
       <c r="P19" s="14"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="N20" s="41" t="s">
+      <c r="N20" s="44" t="s">
         <v>60</v>
       </c>
     </row>
@@ -4160,10 +4142,10 @@
       <c r="F21" s="16">
         <v>200</v>
       </c>
-      <c r="L21" s="38" t="s">
+      <c r="L21" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="N21" s="41"/>
+      <c r="N21" s="44"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -4178,7 +4160,7 @@
       <c r="F22" s="16">
         <v>100</v>
       </c>
-      <c r="L22" s="45"/>
+      <c r="L22" s="42"/>
       <c r="M22" s="10"/>
       <c r="N22" s="14"/>
     </row>
@@ -4192,7 +4174,7 @@
       <c r="F23" s="16">
         <v>40</v>
       </c>
-      <c r="L23" s="37" t="s">
+      <c r="L23" s="38" t="s">
         <v>80</v>
       </c>
     </row>
@@ -4206,7 +4188,7 @@
       <c r="F24" s="16">
         <v>50</v>
       </c>
-      <c r="L24" s="37"/>
+      <c r="L24" s="38"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -4233,7 +4215,7 @@
       <c r="F26" s="16">
         <v>10</v>
       </c>
-      <c r="P26" s="38" t="s">
+      <c r="P26" s="39" t="s">
         <v>123</v>
       </c>
     </row>
@@ -4241,13 +4223,13 @@
       <c r="A27" t="s">
         <v>83</v>
       </c>
-      <c r="P27" s="45"/>
+      <c r="P27" s="42"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>32</v>
       </c>
-      <c r="P28" s="37" t="s">
+      <c r="P28" s="38" t="s">
         <v>60</v>
       </c>
     </row>
@@ -4255,18 +4237,13 @@
       <c r="A29" t="s">
         <v>49</v>
       </c>
-      <c r="P29" s="37"/>
+      <c r="P29" s="38"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C11:J16">
     <sortCondition descending="1" ref="H11:H16"/>
   </sortState>
   <mergeCells count="16">
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="L9:L10"/>
     <mergeCell ref="L23:L24"/>
     <mergeCell ref="P26:P27"/>
     <mergeCell ref="P28:P29"/>
@@ -4278,6 +4255,11 @@
     <mergeCell ref="N20:N21"/>
     <mergeCell ref="L21:L22"/>
     <mergeCell ref="L11:L12"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="L9:L10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4383,7 +4365,7 @@
       <c r="J3" s="1">
         <v>1530.24</v>
       </c>
-      <c r="L3" s="38" t="s">
+      <c r="L3" s="39" t="s">
         <v>138</v>
       </c>
     </row>
@@ -4419,7 +4401,7 @@
       <c r="J4" s="1">
         <v>1530.84</v>
       </c>
-      <c r="L4" s="45"/>
+      <c r="L4" s="42"/>
       <c r="M4" s="10"/>
     </row>
     <row r="5" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4451,7 +4433,7 @@
       <c r="J5">
         <v>1523.86</v>
       </c>
-      <c r="L5" s="39" t="s">
+      <c r="L5" s="40" t="s">
         <v>80</v>
       </c>
       <c r="N5" s="14"/>
@@ -4485,8 +4467,8 @@
       <c r="J6">
         <v>1541.3</v>
       </c>
-      <c r="L6" s="39"/>
-      <c r="N6" s="41" t="s">
+      <c r="L6" s="40"/>
+      <c r="N6" s="44" t="s">
         <v>124</v>
       </c>
     </row>
@@ -4519,7 +4501,7 @@
       <c r="J7">
         <v>1631.78</v>
       </c>
-      <c r="N7" s="46"/>
+      <c r="N7" s="45"/>
       <c r="O7" s="10"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -4552,7 +4534,7 @@
       <c r="J8" s="10">
         <v>1453.8</v>
       </c>
-      <c r="N8" s="42" t="s">
+      <c r="N8" s="43" t="s">
         <v>60</v>
       </c>
       <c r="P8" s="14"/>
@@ -4561,10 +4543,10 @@
       <c r="A9" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="L9" s="37" t="s">
+      <c r="L9" s="38" t="s">
         <v>137</v>
       </c>
-      <c r="N9" s="42"/>
+      <c r="N9" s="43"/>
       <c r="P9" s="14"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -4598,7 +4580,7 @@
       <c r="J10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="L10" s="44"/>
+      <c r="L10" s="46"/>
       <c r="M10" s="10"/>
       <c r="N10" s="14"/>
       <c r="P10" s="14"/>
@@ -4635,7 +4617,7 @@
       <c r="J11" s="1">
         <v>1851.34</v>
       </c>
-      <c r="L11" s="38" t="s">
+      <c r="L11" s="39" t="s">
         <v>60</v>
       </c>
       <c r="P11" s="14"/>
@@ -4672,8 +4654,8 @@
       <c r="J12" s="1">
         <v>1742.32</v>
       </c>
-      <c r="L12" s="38"/>
-      <c r="P12" s="42" t="s">
+      <c r="L12" s="39"/>
+      <c r="P12" s="43" t="s">
         <v>60</v>
       </c>
     </row>
@@ -4709,7 +4691,7 @@
       <c r="J13" s="1">
         <v>1566.5</v>
       </c>
-      <c r="P13" s="43"/>
+      <c r="P13" s="47"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -4743,7 +4725,7 @@
       <c r="J14" s="1">
         <v>1453.92</v>
       </c>
-      <c r="P14" s="41" t="s">
+      <c r="P14" s="44" t="s">
         <v>122</v>
       </c>
     </row>
@@ -4776,10 +4758,10 @@
       <c r="J15">
         <v>1573</v>
       </c>
-      <c r="L15" s="38" t="s">
+      <c r="L15" s="39" t="s">
         <v>135</v>
       </c>
-      <c r="P15" s="41"/>
+      <c r="P15" s="44"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B16">
@@ -4810,12 +4792,12 @@
       <c r="J16">
         <v>1656.98</v>
       </c>
-      <c r="L16" s="45"/>
+      <c r="L16" s="42"/>
       <c r="M16" s="10"/>
       <c r="P16" s="14"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L17" s="37" t="s">
+      <c r="L17" s="38" t="s">
         <v>136</v>
       </c>
       <c r="N17" s="14"/>
@@ -4823,20 +4805,20 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H18" s="4"/>
-      <c r="L18" s="37"/>
-      <c r="N18" s="42" t="s">
+      <c r="L18" s="38"/>
+      <c r="N18" s="43" t="s">
         <v>135</v>
       </c>
       <c r="P18" s="14"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H19" s="4"/>
-      <c r="N19" s="43"/>
+      <c r="N19" s="47"/>
       <c r="O19" s="10"/>
       <c r="P19" s="14"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="N20" s="41" t="s">
+      <c r="N20" s="44" t="s">
         <v>96</v>
       </c>
     </row>
@@ -4850,10 +4832,10 @@
       <c r="F21" s="16">
         <v>200</v>
       </c>
-      <c r="L21" s="38" t="s">
+      <c r="L21" s="39" t="s">
         <v>96</v>
       </c>
-      <c r="N21" s="41"/>
+      <c r="N21" s="44"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -4868,7 +4850,7 @@
       <c r="F22" s="16">
         <v>100</v>
       </c>
-      <c r="L22" s="45"/>
+      <c r="L22" s="42"/>
       <c r="M22" s="10"/>
       <c r="N22" s="14"/>
     </row>
@@ -4882,7 +4864,7 @@
       <c r="F23" s="16">
         <v>40</v>
       </c>
-      <c r="L23" s="37" t="s">
+      <c r="L23" s="38" t="s">
         <v>80</v>
       </c>
     </row>
@@ -4896,7 +4878,7 @@
       <c r="F24" s="16">
         <v>50</v>
       </c>
-      <c r="L24" s="37"/>
+      <c r="L24" s="38"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -4923,7 +4905,7 @@
       <c r="F26" s="16">
         <v>10</v>
       </c>
-      <c r="P26" s="37" t="s">
+      <c r="P26" s="38" t="s">
         <v>124</v>
       </c>
     </row>
@@ -4931,13 +4913,13 @@
       <c r="A27" t="s">
         <v>83</v>
       </c>
-      <c r="P27" s="44"/>
+      <c r="P27" s="46"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>32</v>
       </c>
-      <c r="P28" s="38" t="s">
+      <c r="P28" s="39" t="s">
         <v>96</v>
       </c>
     </row>
@@ -4945,7 +4927,7 @@
       <c r="A29" t="s">
         <v>49</v>
       </c>
-      <c r="P29" s="38"/>
+      <c r="P29" s="39"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
@@ -4957,11 +4939,6 @@
     <sortCondition descending="1" ref="H11:H16"/>
   </sortState>
   <mergeCells count="16">
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="L9:L10"/>
     <mergeCell ref="L23:L24"/>
     <mergeCell ref="P26:P27"/>
     <mergeCell ref="P28:P29"/>
@@ -4973,6 +4950,11 @@
     <mergeCell ref="N20:N21"/>
     <mergeCell ref="L21:L22"/>
     <mergeCell ref="L11:L12"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="L9:L10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5078,7 +5060,7 @@
       <c r="J3" s="1">
         <v>1744.88</v>
       </c>
-      <c r="L3" s="38" t="s">
+      <c r="L3" s="39" t="s">
         <v>136</v>
       </c>
     </row>
@@ -5114,7 +5096,7 @@
       <c r="J4" s="1">
         <v>1652.44</v>
       </c>
-      <c r="L4" s="45"/>
+      <c r="L4" s="42"/>
       <c r="M4" s="10"/>
     </row>
     <row r="5" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5149,7 +5131,7 @@
       <c r="J5" s="1">
         <v>1613.18</v>
       </c>
-      <c r="L5" s="39" t="s">
+      <c r="L5" s="40" t="s">
         <v>80</v>
       </c>
       <c r="N5" s="14"/>
@@ -5183,8 +5165,8 @@
       <c r="J6">
         <v>1612.58</v>
       </c>
-      <c r="L6" s="39"/>
-      <c r="N6" s="42" t="s">
+      <c r="L6" s="40"/>
+      <c r="N6" s="43" t="s">
         <v>136</v>
       </c>
     </row>
@@ -5217,7 +5199,7 @@
       <c r="J7">
         <v>1567.06</v>
       </c>
-      <c r="N7" s="43"/>
+      <c r="N7" s="47"/>
       <c r="O7" s="10"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -5250,7 +5232,7 @@
       <c r="J8" s="10">
         <v>1467.82</v>
       </c>
-      <c r="N8" s="41" t="s">
+      <c r="N8" s="44" t="s">
         <v>142</v>
       </c>
       <c r="P8" s="14"/>
@@ -5259,10 +5241,10 @@
       <c r="A9" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="L9" s="37" t="s">
+      <c r="L9" s="38" t="s">
         <v>143</v>
       </c>
-      <c r="N9" s="41"/>
+      <c r="N9" s="44"/>
       <c r="P9" s="14"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -5296,7 +5278,7 @@
       <c r="J10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="L10" s="44"/>
+      <c r="L10" s="46"/>
       <c r="M10" s="10"/>
       <c r="N10" s="14"/>
       <c r="P10" s="14"/>
@@ -5333,7 +5315,7 @@
       <c r="J11" s="1">
         <v>1764.64</v>
       </c>
-      <c r="L11" s="38" t="s">
+      <c r="L11" s="39" t="s">
         <v>142</v>
       </c>
       <c r="P11" s="14"/>
@@ -5370,8 +5352,8 @@
       <c r="J12" s="1">
         <v>1574.5</v>
       </c>
-      <c r="L12" s="38"/>
-      <c r="P12" s="41" t="s">
+      <c r="L12" s="39"/>
+      <c r="P12" s="44" t="s">
         <v>136</v>
       </c>
     </row>
@@ -5407,7 +5389,7 @@
       <c r="J13" s="1">
         <v>1644.76</v>
       </c>
-      <c r="P13" s="46"/>
+      <c r="P13" s="45"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B14">
@@ -5438,7 +5420,7 @@
       <c r="J14">
         <v>1397.72</v>
       </c>
-      <c r="P14" s="42" t="s">
+      <c r="P14" s="43" t="s">
         <v>118</v>
       </c>
     </row>
@@ -5471,10 +5453,10 @@
       <c r="J15">
         <v>1368.44</v>
       </c>
-      <c r="L15" s="38" t="s">
+      <c r="L15" s="39" t="s">
         <v>118</v>
       </c>
-      <c r="P15" s="42"/>
+      <c r="P15" s="43"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B16">
@@ -5505,12 +5487,12 @@
       <c r="J16">
         <v>1319.8</v>
       </c>
-      <c r="L16" s="45"/>
+      <c r="L16" s="42"/>
       <c r="M16" s="10"/>
       <c r="P16" s="14"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L17" s="37" t="s">
+      <c r="L17" s="38" t="s">
         <v>96</v>
       </c>
       <c r="N17" s="14"/>
@@ -5518,20 +5500,20 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H18" s="4"/>
-      <c r="L18" s="37"/>
-      <c r="N18" s="42" t="s">
+      <c r="L18" s="38"/>
+      <c r="N18" s="43" t="s">
         <v>118</v>
       </c>
       <c r="P18" s="14"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H19" s="4"/>
-      <c r="N19" s="43"/>
+      <c r="N19" s="47"/>
       <c r="O19" s="10"/>
       <c r="P19" s="14"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="N20" s="41" t="s">
+      <c r="N20" s="44" t="s">
         <v>115</v>
       </c>
     </row>
@@ -5545,10 +5527,10 @@
       <c r="F21" s="16">
         <v>200</v>
       </c>
-      <c r="L21" s="38" t="s">
+      <c r="L21" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="N21" s="41"/>
+      <c r="N21" s="44"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
@@ -5563,7 +5545,7 @@
       <c r="F22" s="16">
         <v>100</v>
       </c>
-      <c r="L22" s="45"/>
+      <c r="L22" s="42"/>
       <c r="M22" s="10"/>
       <c r="N22" s="14"/>
     </row>
@@ -5578,7 +5560,7 @@
       <c r="F23" s="16">
         <v>40</v>
       </c>
-      <c r="L23" s="37" t="s">
+      <c r="L23" s="38" t="s">
         <v>80</v>
       </c>
     </row>
@@ -5593,7 +5575,7 @@
       <c r="F24" s="16">
         <v>50</v>
       </c>
-      <c r="L24" s="37"/>
+      <c r="L24" s="38"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
@@ -5622,7 +5604,7 @@
       <c r="F26" s="16">
         <v>10</v>
       </c>
-      <c r="P26" s="37" t="s">
+      <c r="P26" s="38" t="s">
         <v>142</v>
       </c>
     </row>
@@ -5631,14 +5613,14 @@
         <v>83</v>
       </c>
       <c r="B27" s="5"/>
-      <c r="P27" s="44"/>
+      <c r="P27" s="46"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B28" s="5"/>
-      <c r="P28" s="38" t="s">
+      <c r="P28" s="39" t="s">
         <v>115</v>
       </c>
     </row>
@@ -5647,7 +5629,7 @@
         <v>49</v>
       </c>
       <c r="B29" s="5"/>
-      <c r="P29" s="38"/>
+      <c r="P29" s="39"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
@@ -5660,11 +5642,6 @@
     <sortCondition descending="1" ref="H11:H16"/>
   </sortState>
   <mergeCells count="16">
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="L9:L10"/>
     <mergeCell ref="L23:L24"/>
     <mergeCell ref="P26:P27"/>
     <mergeCell ref="P28:P29"/>
@@ -5676,6 +5653,11 @@
     <mergeCell ref="N20:N21"/>
     <mergeCell ref="L21:L22"/>
     <mergeCell ref="L11:L12"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="L9:L10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5799,7 +5781,7 @@
       <c r="I3" s="1">
         <v>1830.48</v>
       </c>
-      <c r="K3" s="38" t="s">
+      <c r="K3" s="39" t="s">
         <v>147</v>
       </c>
     </row>
@@ -5832,7 +5814,7 @@
       <c r="I4" s="1">
         <v>1957.51</v>
       </c>
-      <c r="K4" s="45"/>
+      <c r="K4" s="42"/>
       <c r="L4" s="10"/>
     </row>
     <row r="5" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5864,7 +5846,7 @@
       <c r="I5" s="1">
         <v>2011.64</v>
       </c>
-      <c r="K5" s="39" t="s">
+      <c r="K5" s="40" t="s">
         <v>80</v>
       </c>
       <c r="M5" s="14"/>
@@ -5898,8 +5880,8 @@
       <c r="I6" s="1">
         <v>1810.54</v>
       </c>
-      <c r="K6" s="39"/>
-      <c r="M6" s="41" t="s">
+      <c r="K6" s="40"/>
+      <c r="M6" s="44" t="s">
         <v>147</v>
       </c>
     </row>
@@ -5932,7 +5914,7 @@
       <c r="I7" s="1">
         <v>1739.8</v>
       </c>
-      <c r="M7" s="46"/>
+      <c r="M7" s="45"/>
       <c r="N7" s="10"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -5961,7 +5943,7 @@
       <c r="I8">
         <v>1557.34</v>
       </c>
-      <c r="M8" s="42" t="s">
+      <c r="M8" s="43" t="s">
         <v>115</v>
       </c>
       <c r="O8" s="14"/>
@@ -5992,10 +5974,10 @@
       <c r="I9">
         <v>1632.8</v>
       </c>
-      <c r="K9" s="38" t="s">
+      <c r="K9" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="M9" s="42"/>
+      <c r="M9" s="43"/>
       <c r="O9" s="14"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -6024,7 +6006,7 @@
       <c r="I10">
         <v>1479.68</v>
       </c>
-      <c r="K10" s="45"/>
+      <c r="K10" s="42"/>
       <c r="L10" s="10"/>
       <c r="M10" s="14"/>
       <c r="O10" s="14"/>
@@ -6055,7 +6037,7 @@
       <c r="I11">
         <v>1326.38</v>
       </c>
-      <c r="K11" s="37" t="s">
+      <c r="K11" s="38" t="s">
         <v>136</v>
       </c>
       <c r="O11" s="14"/>
@@ -6086,8 +6068,8 @@
       <c r="I12">
         <v>1491.86</v>
       </c>
-      <c r="K12" s="37"/>
-      <c r="O12" s="42" t="s">
+      <c r="K12" s="38"/>
+      <c r="O12" s="43" t="s">
         <v>115</v>
       </c>
     </row>
@@ -6117,29 +6099,29 @@
       <c r="I13">
         <v>1391.5</v>
       </c>
-      <c r="O13" s="43"/>
+      <c r="O13" s="47"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H14" s="4"/>
-      <c r="O14" s="41" t="s">
+      <c r="O14" s="44" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H15" s="4"/>
-      <c r="K15" s="38" t="s">
+      <c r="K15" s="39" t="s">
         <v>145</v>
       </c>
-      <c r="O15" s="41"/>
+      <c r="O15" s="44"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H16" s="4"/>
-      <c r="K16" s="45"/>
+      <c r="K16" s="42"/>
       <c r="L16" s="10"/>
       <c r="O16" s="14"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="K17" s="37" t="s">
+      <c r="K17" s="38" t="s">
         <v>99</v>
       </c>
       <c r="M17" s="14"/>
@@ -6147,20 +6129,20 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H18" s="4"/>
-      <c r="K18" s="37"/>
-      <c r="M18" s="42" t="s">
+      <c r="K18" s="38"/>
+      <c r="M18" s="43" t="s">
         <v>145</v>
       </c>
       <c r="O18" s="14"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H19" s="4"/>
-      <c r="M19" s="43"/>
+      <c r="M19" s="47"/>
       <c r="N19" s="10"/>
       <c r="O19" s="14"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="M20" s="47" t="s">
+      <c r="M20" s="48" t="s">
         <v>154</v>
       </c>
     </row>
@@ -6174,10 +6156,10 @@
       <c r="F21" s="16">
         <v>200</v>
       </c>
-      <c r="K21" s="38" t="s">
+      <c r="K21" s="39" t="s">
         <v>154</v>
       </c>
-      <c r="M21" s="41"/>
+      <c r="M21" s="44"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
@@ -6192,7 +6174,7 @@
       <c r="F22" s="16">
         <v>100</v>
       </c>
-      <c r="K22" s="45"/>
+      <c r="K22" s="42"/>
       <c r="L22" s="10"/>
       <c r="M22" s="14"/>
     </row>
@@ -6207,7 +6189,7 @@
       <c r="F23" s="17">
         <v>30</v>
       </c>
-      <c r="K23" s="37" t="s">
+      <c r="K23" s="38" t="s">
         <v>80</v>
       </c>
     </row>
@@ -6222,7 +6204,7 @@
       <c r="F24" s="16">
         <v>50</v>
       </c>
-      <c r="K24" s="37"/>
+      <c r="K24" s="38"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
@@ -6251,7 +6233,7 @@
       <c r="F26" s="16">
         <v>10</v>
       </c>
-      <c r="O26" s="37" t="s">
+      <c r="O26" s="38" t="s">
         <v>147</v>
       </c>
     </row>
@@ -6260,14 +6242,14 @@
         <v>83</v>
       </c>
       <c r="B27" s="5"/>
-      <c r="O27" s="44"/>
+      <c r="O27" s="46"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B28" s="5"/>
-      <c r="O28" s="38" t="s">
+      <c r="O28" s="39" t="s">
         <v>154</v>
       </c>
     </row>
@@ -6276,7 +6258,7 @@
         <v>49</v>
       </c>
       <c r="B29" s="5"/>
-      <c r="O29" s="38"/>
+      <c r="O29" s="39"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
@@ -6289,11 +6271,6 @@
     <sortCondition descending="1" ref="H2:H13"/>
   </sortState>
   <mergeCells count="16">
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="K9:K10"/>
     <mergeCell ref="K23:K24"/>
     <mergeCell ref="O26:O27"/>
     <mergeCell ref="O28:O29"/>
@@ -6305,6 +6282,11 @@
     <mergeCell ref="M20:M21"/>
     <mergeCell ref="K21:K22"/>
     <mergeCell ref="K11:K12"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="K9:K10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6428,7 +6410,7 @@
       <c r="I3" s="1">
         <v>1668.12</v>
       </c>
-      <c r="K3" s="38" t="s">
+      <c r="K3" s="39" t="s">
         <v>152</v>
       </c>
     </row>
@@ -6461,7 +6443,7 @@
       <c r="I4" s="1">
         <v>1799.34</v>
       </c>
-      <c r="K4" s="45"/>
+      <c r="K4" s="42"/>
       <c r="L4" s="10"/>
     </row>
     <row r="5" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6493,7 +6475,7 @@
       <c r="I5" s="1">
         <v>1912.76</v>
       </c>
-      <c r="K5" s="39" t="s">
+      <c r="K5" s="40" t="s">
         <v>80</v>
       </c>
       <c r="M5" s="14"/>
@@ -6527,8 +6509,8 @@
       <c r="I6" s="1">
         <v>1688.86</v>
       </c>
-      <c r="K6" s="39"/>
-      <c r="M6" s="41" t="s">
+      <c r="K6" s="40"/>
+      <c r="M6" s="44" t="s">
         <v>152</v>
       </c>
     </row>
@@ -6561,7 +6543,7 @@
       <c r="I7" s="1">
         <v>1626.76</v>
       </c>
-      <c r="M7" s="46"/>
+      <c r="M7" s="45"/>
       <c r="N7" s="10"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -6590,7 +6572,7 @@
       <c r="I8">
         <v>1557.08</v>
       </c>
-      <c r="M8" s="42" t="s">
+      <c r="M8" s="43" t="s">
         <v>146</v>
       </c>
       <c r="O8" s="14"/>
@@ -6621,10 +6603,10 @@
       <c r="I9">
         <v>1554.84</v>
       </c>
-      <c r="K9" s="38" t="s">
+      <c r="K9" s="39" t="s">
         <v>154</v>
       </c>
-      <c r="M9" s="42"/>
+      <c r="M9" s="43"/>
       <c r="O9" s="14"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -6653,7 +6635,7 @@
       <c r="I10">
         <v>1463.02</v>
       </c>
-      <c r="K10" s="45"/>
+      <c r="K10" s="42"/>
       <c r="L10" s="10"/>
       <c r="M10" s="14"/>
       <c r="O10" s="14"/>
@@ -6684,7 +6666,7 @@
       <c r="I11">
         <v>1798.06</v>
       </c>
-      <c r="K11" s="37" t="s">
+      <c r="K11" s="38" t="s">
         <v>118</v>
       </c>
       <c r="O11" s="14"/>
@@ -6715,8 +6697,8 @@
       <c r="I12">
         <v>1635.74</v>
       </c>
-      <c r="K12" s="37"/>
-      <c r="O12" s="42" t="s">
+      <c r="K12" s="38"/>
+      <c r="O12" s="43" t="s">
         <v>154</v>
       </c>
     </row>
@@ -6746,29 +6728,29 @@
       <c r="I13">
         <v>1620.5</v>
       </c>
-      <c r="O13" s="43"/>
+      <c r="O13" s="47"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H14" s="4"/>
-      <c r="O14" s="41" t="s">
+      <c r="O14" s="44" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H15" s="4"/>
-      <c r="K15" s="37" t="s">
+      <c r="K15" s="38" t="s">
         <v>145</v>
       </c>
-      <c r="O15" s="41"/>
+      <c r="O15" s="44"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H16" s="4"/>
-      <c r="K16" s="44"/>
+      <c r="K16" s="46"/>
       <c r="L16" s="10"/>
       <c r="O16" s="14"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="K17" s="38" t="s">
+      <c r="K17" s="39" t="s">
         <v>60</v>
       </c>
       <c r="M17" s="14"/>
@@ -6776,20 +6758,20 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H18" s="4"/>
-      <c r="K18" s="38"/>
-      <c r="M18" s="41" t="s">
+      <c r="K18" s="39"/>
+      <c r="M18" s="44" t="s">
         <v>60</v>
       </c>
       <c r="O18" s="14"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H19" s="4"/>
-      <c r="M19" s="46"/>
+      <c r="M19" s="45"/>
       <c r="N19" s="10"/>
       <c r="O19" s="14"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="M20" s="48" t="s">
+      <c r="M20" s="49" t="s">
         <v>151</v>
       </c>
     </row>
@@ -6803,10 +6785,10 @@
       <c r="F21" s="16">
         <v>200</v>
       </c>
-      <c r="K21" s="38" t="s">
+      <c r="K21" s="39" t="s">
         <v>151</v>
       </c>
-      <c r="M21" s="42"/>
+      <c r="M21" s="43"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
@@ -6821,7 +6803,7 @@
       <c r="F22" s="16">
         <v>100</v>
       </c>
-      <c r="K22" s="45"/>
+      <c r="K22" s="42"/>
       <c r="L22" s="10"/>
       <c r="M22" s="14"/>
     </row>
@@ -6836,7 +6818,7 @@
       <c r="F23" s="16">
         <v>30</v>
       </c>
-      <c r="K23" s="37" t="s">
+      <c r="K23" s="38" t="s">
         <v>80</v>
       </c>
     </row>
@@ -6851,7 +6833,7 @@
       <c r="F24" s="16">
         <v>50</v>
       </c>
-      <c r="K24" s="37"/>
+      <c r="K24" s="38"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
@@ -6880,7 +6862,7 @@
       <c r="F26" s="16">
         <v>10</v>
       </c>
-      <c r="O26" s="38" t="s">
+      <c r="O26" s="39" t="s">
         <v>152</v>
       </c>
     </row>
@@ -6889,7 +6871,7 @@
         <v>83</v>
       </c>
       <c r="B27" s="5"/>
-      <c r="O27" s="45"/>
+      <c r="O27" s="42"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
@@ -6899,7 +6881,7 @@
       <c r="C28" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="O28" s="37" t="s">
+      <c r="O28" s="38" t="s">
         <v>60</v>
       </c>
     </row>
@@ -6908,7 +6890,7 @@
         <v>49</v>
       </c>
       <c r="B29" s="5"/>
-      <c r="O29" s="37"/>
+      <c r="O29" s="38"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
@@ -6921,11 +6903,6 @@
     <sortCondition descending="1" ref="H2:H13"/>
   </sortState>
   <mergeCells count="16">
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="K9:K10"/>
     <mergeCell ref="K23:K24"/>
     <mergeCell ref="O26:O27"/>
     <mergeCell ref="O28:O29"/>
@@ -6937,6 +6914,11 @@
     <mergeCell ref="M20:M21"/>
     <mergeCell ref="K21:K22"/>
     <mergeCell ref="K11:K12"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="K9:K10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7060,7 +7042,7 @@
       <c r="I3" s="1">
         <v>1879.82</v>
       </c>
-      <c r="K3" s="38" t="s">
+      <c r="K3" s="39" t="s">
         <v>155</v>
       </c>
     </row>
@@ -7093,7 +7075,7 @@
       <c r="I4" s="1">
         <v>1689.34</v>
       </c>
-      <c r="K4" s="45"/>
+      <c r="K4" s="42"/>
       <c r="L4" s="10"/>
     </row>
     <row r="5" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7125,7 +7107,7 @@
       <c r="I5" s="1">
         <v>1702.92</v>
       </c>
-      <c r="K5" s="39" t="s">
+      <c r="K5" s="40" t="s">
         <v>80</v>
       </c>
       <c r="M5" s="14"/>
@@ -7159,8 +7141,8 @@
       <c r="I6" s="1">
         <v>1695.94</v>
       </c>
-      <c r="K6" s="39"/>
-      <c r="M6" s="42" t="s">
+      <c r="K6" s="40"/>
+      <c r="M6" s="43" t="s">
         <v>155</v>
       </c>
     </row>
@@ -7193,7 +7175,7 @@
       <c r="I7" s="1">
         <v>1633.82</v>
       </c>
-      <c r="M7" s="43"/>
+      <c r="M7" s="47"/>
       <c r="N7" s="10"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -7222,7 +7204,7 @@
       <c r="I8">
         <v>1591.5</v>
       </c>
-      <c r="M8" s="41" t="s">
+      <c r="M8" s="44" t="s">
         <v>147</v>
       </c>
       <c r="O8" s="14"/>
@@ -7253,10 +7235,10 @@
       <c r="I9">
         <v>1566.6</v>
       </c>
-      <c r="K9" s="37" t="s">
+      <c r="K9" s="38" t="s">
         <v>156</v>
       </c>
-      <c r="M9" s="41"/>
+      <c r="M9" s="44"/>
       <c r="O9" s="14"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -7285,7 +7267,7 @@
       <c r="I10">
         <v>1757.42</v>
       </c>
-      <c r="K10" s="44"/>
+      <c r="K10" s="46"/>
       <c r="L10" s="10"/>
       <c r="M10" s="14"/>
       <c r="O10" s="14"/>
@@ -7316,7 +7298,7 @@
       <c r="I11">
         <v>1740</v>
       </c>
-      <c r="K11" s="38" t="s">
+      <c r="K11" s="39" t="s">
         <v>147</v>
       </c>
       <c r="O11" s="14"/>
@@ -7347,8 +7329,8 @@
       <c r="I12">
         <v>1435.98</v>
       </c>
-      <c r="K12" s="38"/>
-      <c r="O12" s="41" t="s">
+      <c r="K12" s="39"/>
+      <c r="O12" s="44" t="s">
         <v>155</v>
       </c>
     </row>
@@ -7378,29 +7360,29 @@
       <c r="I13">
         <v>1443.12</v>
       </c>
-      <c r="O13" s="46"/>
+      <c r="O13" s="45"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H14" s="4"/>
-      <c r="O14" s="42" t="s">
+      <c r="O14" s="43" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H15" s="4"/>
-      <c r="K15" s="38" t="s">
+      <c r="K15" s="39" t="s">
         <v>145</v>
       </c>
-      <c r="O15" s="42"/>
+      <c r="O15" s="43"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H16" s="4"/>
-      <c r="K16" s="45"/>
+      <c r="K16" s="42"/>
       <c r="L16" s="10"/>
       <c r="O16" s="14"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="K17" s="37" t="s">
+      <c r="K17" s="38" t="s">
         <v>148</v>
       </c>
       <c r="M17" s="14"/>
@@ -7408,20 +7390,20 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H18" s="4"/>
-      <c r="K18" s="37"/>
-      <c r="M18" s="41" t="s">
+      <c r="K18" s="38"/>
+      <c r="M18" s="44" t="s">
         <v>145</v>
       </c>
       <c r="O18" s="14"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H19" s="4"/>
-      <c r="M19" s="46"/>
+      <c r="M19" s="45"/>
       <c r="N19" s="10"/>
       <c r="O19" s="14"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="M20" s="48" t="s">
+      <c r="M20" s="49" t="s">
         <v>137</v>
       </c>
     </row>
@@ -7435,10 +7417,10 @@
       <c r="F21" s="16">
         <v>200</v>
       </c>
-      <c r="K21" s="38" t="s">
+      <c r="K21" s="39" t="s">
         <v>137</v>
       </c>
-      <c r="M21" s="42"/>
+      <c r="M21" s="43"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
@@ -7453,7 +7435,7 @@
       <c r="F22" s="16">
         <v>100</v>
       </c>
-      <c r="K22" s="45"/>
+      <c r="K22" s="42"/>
       <c r="L22" s="10"/>
       <c r="M22" s="14"/>
     </row>
@@ -7468,7 +7450,7 @@
       <c r="F23" s="16">
         <v>30</v>
       </c>
-      <c r="K23" s="37" t="s">
+      <c r="K23" s="38" t="s">
         <v>80</v>
       </c>
     </row>
@@ -7483,7 +7465,7 @@
       <c r="F24" s="16">
         <v>50</v>
       </c>
-      <c r="K24" s="37"/>
+      <c r="K24" s="38"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
@@ -7512,7 +7494,7 @@
       <c r="F26" s="16">
         <v>10</v>
       </c>
-      <c r="O26" s="38" t="s">
+      <c r="O26" s="39" t="s">
         <v>147</v>
       </c>
     </row>
@@ -7521,7 +7503,7 @@
         <v>83</v>
       </c>
       <c r="B27" s="5"/>
-      <c r="O27" s="45"/>
+      <c r="O27" s="42"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
@@ -7531,7 +7513,7 @@
       <c r="C28" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="O28" s="37" t="s">
+      <c r="O28" s="38" t="s">
         <v>145</v>
       </c>
     </row>
@@ -7540,7 +7522,7 @@
         <v>49</v>
       </c>
       <c r="B29" s="5"/>
-      <c r="O29" s="37"/>
+      <c r="O29" s="38"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
@@ -7553,11 +7535,6 @@
     <sortCondition descending="1" ref="H2:H13"/>
   </sortState>
   <mergeCells count="16">
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="K9:K10"/>
     <mergeCell ref="K23:K24"/>
     <mergeCell ref="O26:O27"/>
     <mergeCell ref="O28:O29"/>
@@ -7569,6 +7546,11 @@
     <mergeCell ref="M20:M21"/>
     <mergeCell ref="K21:K22"/>
     <mergeCell ref="K11:K12"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="K9:K10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7578,8 +7560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DC38AAB-96CB-42DE-9F89-BEE07C09AAC6}">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18:M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7688,7 +7670,7 @@
       <c r="I3" s="1">
         <v>1810.84</v>
       </c>
-      <c r="K3" s="38" t="s">
+      <c r="K3" s="39" t="s">
         <v>147</v>
       </c>
     </row>
@@ -7719,7 +7701,7 @@
       <c r="I4" s="1">
         <v>1781.88</v>
       </c>
-      <c r="K4" s="45"/>
+      <c r="K4" s="42"/>
       <c r="L4" s="10"/>
     </row>
     <row r="5" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7749,7 +7731,7 @@
       <c r="I5" s="1">
         <v>1758.24</v>
       </c>
-      <c r="K5" s="39" t="s">
+      <c r="K5" s="40" t="s">
         <v>80</v>
       </c>
       <c r="M5" s="14"/>
@@ -7781,8 +7763,8 @@
       <c r="I6" s="1">
         <v>1712.9</v>
       </c>
-      <c r="K6" s="39"/>
-      <c r="M6" s="52" t="s">
+      <c r="K6" s="40"/>
+      <c r="M6" s="44" t="s">
         <v>147</v>
       </c>
     </row>
@@ -7813,7 +7795,7 @@
       <c r="I7" s="1">
         <v>1821.42</v>
       </c>
-      <c r="M7" s="53"/>
+      <c r="M7" s="45"/>
       <c r="N7" s="10"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -7842,7 +7824,9 @@
       <c r="I8">
         <v>1771.9</v>
       </c>
-      <c r="M8" s="41"/>
+      <c r="M8" s="44" t="s">
+        <v>276</v>
+      </c>
       <c r="O8" s="14"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -7871,10 +7855,10 @@
       <c r="I9">
         <v>1582.7</v>
       </c>
-      <c r="K9" s="37" t="s">
+      <c r="K9" s="39" t="s">
         <v>276</v>
       </c>
-      <c r="M9" s="41"/>
+      <c r="M9" s="44"/>
       <c r="O9" s="14"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -7903,7 +7887,7 @@
       <c r="I10">
         <v>1709.36</v>
       </c>
-      <c r="K10" s="44"/>
+      <c r="K10" s="42"/>
       <c r="L10" s="10"/>
       <c r="M10" s="14"/>
       <c r="O10" s="14"/>
@@ -7934,7 +7918,7 @@
       <c r="I11">
         <v>1628.92</v>
       </c>
-      <c r="K11" s="49" t="s">
+      <c r="K11" s="38" t="s">
         <v>60</v>
       </c>
       <c r="O11" s="14"/>
@@ -7965,8 +7949,8 @@
       <c r="I12">
         <v>1418.44</v>
       </c>
-      <c r="K12" s="49"/>
-      <c r="O12" s="41"/>
+      <c r="K12" s="38"/>
+      <c r="O12" s="44"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B13">
@@ -7994,27 +7978,27 @@
       <c r="I13">
         <v>1315.52</v>
       </c>
-      <c r="O13" s="46"/>
+      <c r="O13" s="45"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H14" s="4"/>
-      <c r="O14" s="52"/>
+      <c r="O14" s="44"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H15" s="4"/>
-      <c r="K15" s="49" t="s">
+      <c r="K15" s="39" t="s">
         <v>145</v>
       </c>
-      <c r="O15" s="52"/>
+      <c r="O15" s="44"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H16" s="4"/>
-      <c r="K16" s="50"/>
+      <c r="K16" s="42"/>
       <c r="L16" s="10"/>
       <c r="O16" s="14"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="K17" s="37" t="s">
+      <c r="K17" s="38" t="s">
         <v>155</v>
       </c>
       <c r="M17" s="14"/>
@@ -8022,18 +8006,20 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H18" s="4"/>
-      <c r="K18" s="37"/>
-      <c r="M18" s="41"/>
+      <c r="K18" s="38"/>
+      <c r="M18" s="44" t="s">
+        <v>145</v>
+      </c>
       <c r="O18" s="14"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H19" s="4"/>
-      <c r="M19" s="46"/>
+      <c r="M19" s="45"/>
       <c r="N19" s="10"/>
       <c r="O19" s="14"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="M20" s="51" t="s">
+      <c r="M20" s="48" t="s">
         <v>273</v>
       </c>
     </row>
@@ -8047,10 +8033,10 @@
       <c r="F21" s="16">
         <v>200</v>
       </c>
-      <c r="K21" s="38" t="s">
+      <c r="K21" s="39" t="s">
         <v>273</v>
       </c>
-      <c r="M21" s="52"/>
+      <c r="M21" s="44"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
@@ -8065,7 +8051,7 @@
       <c r="F22" s="16">
         <v>100</v>
       </c>
-      <c r="K22" s="45"/>
+      <c r="K22" s="42"/>
       <c r="L22" s="10"/>
       <c r="M22" s="14"/>
     </row>
@@ -8080,7 +8066,7 @@
       <c r="F23" s="16">
         <v>30</v>
       </c>
-      <c r="K23" s="37" t="s">
+      <c r="K23" s="38" t="s">
         <v>80</v>
       </c>
     </row>
@@ -8095,7 +8081,7 @@
       <c r="F24" s="16">
         <v>50</v>
       </c>
-      <c r="K24" s="37"/>
+      <c r="K24" s="38"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
@@ -8124,14 +8110,14 @@
       <c r="F26" s="16">
         <v>10</v>
       </c>
-      <c r="O26" s="49"/>
+      <c r="O26" s="38"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>83</v>
       </c>
       <c r="B27" s="5"/>
-      <c r="O27" s="50"/>
+      <c r="O27" s="46"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
@@ -8141,14 +8127,14 @@
       <c r="C28" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="O28" s="37"/>
+      <c r="O28" s="38"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>49</v>
       </c>
       <c r="B29" s="5"/>
-      <c r="O29" s="37"/>
+      <c r="O29" s="38"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
@@ -8158,11 +8144,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="K9:K10"/>
     <mergeCell ref="K23:K24"/>
     <mergeCell ref="O26:O27"/>
     <mergeCell ref="O28:O29"/>
@@ -8174,6 +8155,11 @@
     <mergeCell ref="M20:M21"/>
     <mergeCell ref="K21:K22"/>
     <mergeCell ref="K11:K12"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="K9:K10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8184,7 +8170,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5B52E80-2A72-48E8-8AE2-03BD1ED3BA86}">
   <dimension ref="A1:AU81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="AW7" sqref="AW7"/>
     </sheetView>
   </sheetViews>
@@ -8315,7 +8301,7 @@
       <c r="AN1" s="6">
         <v>2022</v>
       </c>
-      <c r="AO1" s="54">
+      <c r="AO1" s="6">
         <v>2023</v>
       </c>
       <c r="AP1" s="33">
@@ -8480,7 +8466,7 @@
         <f>_xlfn.XLOOKUP($A2,'2022'!$D$2:$D$13,'2022'!$A$2:$A$13,"x")</f>
         <v>6</v>
       </c>
-      <c r="AO2" s="55">
+      <c r="AO2">
         <f>_xlfn.XLOOKUP($A2,'2023'!$D$2:$D$13,'2023'!$A$2:$A$13,"x")</f>
         <v>4</v>
       </c>
@@ -8652,7 +8638,7 @@
         <f>_xlfn.XLOOKUP($A3,'2022'!$D$2:$D$13,'2022'!$A$2:$A$13,"x")</f>
         <v>x</v>
       </c>
-      <c r="AO3" s="56" t="str">
+      <c r="AO3" s="37" t="str">
         <f>_xlfn.XLOOKUP($A3,'2023'!$D$2:$D$13,'2023'!$A$2:$A$13,"x")</f>
         <v>x</v>
       </c>
@@ -8824,7 +8810,7 @@
         <f>_xlfn.XLOOKUP($A4,'2022'!$D$2:$D$13,'2022'!$A$2:$A$13,"x")</f>
         <v>3</v>
       </c>
-      <c r="AO4" s="55">
+      <c r="AO4">
         <f>_xlfn.XLOOKUP($A4,'2023'!$D$2:$D$13,'2023'!$A$2:$A$13,"x")</f>
         <v>0</v>
       </c>
@@ -8996,7 +8982,7 @@
         <f>_xlfn.XLOOKUP($A5,'2022'!$D$2:$D$13,'2022'!$A$2:$A$13,"x")</f>
         <v>x</v>
       </c>
-      <c r="AO5" s="56" t="str">
+      <c r="AO5" s="37" t="str">
         <f>_xlfn.XLOOKUP($A5,'2023'!$D$2:$D$13,'2023'!$A$2:$A$13,"x")</f>
         <v>x</v>
       </c>
@@ -9168,7 +9154,7 @@
         <f>_xlfn.XLOOKUP($A6,'2022'!$D$2:$D$13,'2022'!$A$2:$A$13,"x")</f>
         <v>0</v>
       </c>
-      <c r="AO6" s="55">
+      <c r="AO6">
         <f>_xlfn.XLOOKUP($A6,'2023'!$D$2:$D$13,'2023'!$A$2:$A$13,"x")</f>
         <v>0</v>
       </c>
@@ -9340,7 +9326,7 @@
         <f>_xlfn.XLOOKUP($A7,'2022'!$D$2:$D$13,'2022'!$A$2:$A$13,"x")</f>
         <v>x</v>
       </c>
-      <c r="AO7" s="56" t="str">
+      <c r="AO7" s="37" t="str">
         <f>_xlfn.XLOOKUP($A7,'2023'!$D$2:$D$13,'2023'!$A$2:$A$13,"x")</f>
         <v>x</v>
       </c>
@@ -9512,7 +9498,7 @@
         <f>_xlfn.XLOOKUP($A8,'2022'!$D$2:$D$13,'2022'!$A$2:$A$13,"x")</f>
         <v>x</v>
       </c>
-      <c r="AO8" s="56" t="str">
+      <c r="AO8" s="37" t="str">
         <f>_xlfn.XLOOKUP($A8,'2023'!$D$2:$D$13,'2023'!$A$2:$A$13,"x")</f>
         <v>x</v>
       </c>
@@ -9684,7 +9670,7 @@
         <f>_xlfn.XLOOKUP($A9,'2022'!$D$2:$D$13,'2022'!$A$2:$A$13,"x")</f>
         <v>0</v>
       </c>
-      <c r="AO9" s="55">
+      <c r="AO9">
         <f>_xlfn.XLOOKUP($A9,'2023'!$D$2:$D$13,'2023'!$A$2:$A$13,"x")</f>
         <v>3</v>
       </c>
@@ -9856,7 +9842,7 @@
         <f>_xlfn.XLOOKUP($A10,'2022'!$D$2:$D$13,'2022'!$A$2:$A$13,"x")</f>
         <v>x</v>
       </c>
-      <c r="AO10" s="56" t="str">
+      <c r="AO10" s="37" t="str">
         <f>_xlfn.XLOOKUP($A10,'2023'!$D$2:$D$13,'2023'!$A$2:$A$13,"x")</f>
         <v>x</v>
       </c>
@@ -10028,7 +10014,7 @@
         <f>_xlfn.XLOOKUP($A11,'2022'!$D$2:$D$13,'2022'!$A$2:$A$13,"x")</f>
         <v>2</v>
       </c>
-      <c r="AO11" s="55">
+      <c r="AO11">
         <f>_xlfn.XLOOKUP($A11,'2023'!$D$2:$D$13,'2023'!$A$2:$A$13,"x")</f>
         <v>0</v>
       </c>
@@ -10200,7 +10186,7 @@
         <f>_xlfn.XLOOKUP($A12,'2022'!$D$2:$D$13,'2022'!$A$2:$A$13,"x")</f>
         <v>5</v>
       </c>
-      <c r="AO12" s="55">
+      <c r="AO12">
         <f>_xlfn.XLOOKUP($A12,'2023'!$D$2:$D$13,'2023'!$A$2:$A$13,"x")</f>
         <v>0</v>
       </c>
@@ -10372,7 +10358,7 @@
         <f>_xlfn.XLOOKUP($A13,'2022'!$D$2:$D$13,'2022'!$A$2:$A$13,"x")</f>
         <v>1</v>
       </c>
-      <c r="AO13" s="55">
+      <c r="AO13">
         <f>_xlfn.XLOOKUP($A13,'2023'!$D$2:$D$13,'2023'!$A$2:$A$13,"x")</f>
         <v>0</v>
       </c>
@@ -10544,7 +10530,7 @@
         <f>_xlfn.XLOOKUP($A14,'2022'!$D$2:$D$13,'2022'!$A$2:$A$13,"x")</f>
         <v>4</v>
       </c>
-      <c r="AO14" s="55">
+      <c r="AO14">
         <f>_xlfn.XLOOKUP($A14,'2023'!$D$2:$D$13,'2023'!$A$2:$A$13,"x")</f>
         <v>0</v>
       </c>
@@ -10716,7 +10702,7 @@
         <f>_xlfn.XLOOKUP($A15,'2022'!$D$2:$D$13,'2022'!$A$2:$A$13,"x")</f>
         <v>x</v>
       </c>
-      <c r="AO15" s="56" t="str">
+      <c r="AO15" s="37" t="str">
         <f>_xlfn.XLOOKUP($A15,'2023'!$D$2:$D$13,'2023'!$A$2:$A$13,"x")</f>
         <v>x</v>
       </c>
@@ -10888,7 +10874,7 @@
         <f>_xlfn.XLOOKUP($A16,'2022'!$D$2:$D$13,'2022'!$A$2:$A$13,"x")</f>
         <v>x</v>
       </c>
-      <c r="AO16" s="56" t="str">
+      <c r="AO16" s="37" t="str">
         <f>_xlfn.XLOOKUP($A16,'2023'!$D$2:$D$13,'2023'!$A$2:$A$13,"x")</f>
         <v>x</v>
       </c>
@@ -11060,7 +11046,7 @@
         <f>_xlfn.XLOOKUP($A17,'2022'!$D$2:$D$13,'2022'!$A$2:$A$13,"x")</f>
         <v>x</v>
       </c>
-      <c r="AO17" s="56" t="str">
+      <c r="AO17" s="37" t="str">
         <f>_xlfn.XLOOKUP($A17,'2023'!$D$2:$D$13,'2023'!$A$2:$A$13,"x")</f>
         <v>x</v>
       </c>
@@ -11232,7 +11218,7 @@
         <f>_xlfn.XLOOKUP($A18,'2022'!$D$2:$D$13,'2022'!$A$2:$A$13,"x")</f>
         <v>0</v>
       </c>
-      <c r="AO18" s="55">
+      <c r="AO18">
         <f>_xlfn.XLOOKUP($A18,'2023'!$D$2:$D$13,'2023'!$A$2:$A$13,"x")</f>
         <v>5</v>
       </c>
@@ -11404,7 +11390,7 @@
         <f>_xlfn.XLOOKUP($A19,'2022'!$D$2:$D$13,'2022'!$A$2:$A$13,"x")</f>
         <v>0</v>
       </c>
-      <c r="AO19" s="55">
+      <c r="AO19">
         <f>_xlfn.XLOOKUP($A19,'2023'!$D$2:$D$13,'2023'!$A$2:$A$13,"x")</f>
         <v>1</v>
       </c>
@@ -11576,7 +11562,7 @@
         <f>_xlfn.XLOOKUP($A20,'2022'!$D$2:$D$13,'2022'!$A$2:$A$13,"x")</f>
         <v>x</v>
       </c>
-      <c r="AO20" s="56" t="str">
+      <c r="AO20" s="37" t="str">
         <f>_xlfn.XLOOKUP($A20,'2023'!$D$2:$D$13,'2023'!$A$2:$A$13,"x")</f>
         <v>x</v>
       </c>
@@ -11748,7 +11734,7 @@
         <f>_xlfn.XLOOKUP($A21,'2022'!$D$2:$D$13,'2022'!$A$2:$A$13,"x")</f>
         <v>x</v>
       </c>
-      <c r="AO21" s="56" t="str">
+      <c r="AO21" s="37" t="str">
         <f>_xlfn.XLOOKUP($A21,'2023'!$D$2:$D$13,'2023'!$A$2:$A$13,"x")</f>
         <v>x</v>
       </c>
@@ -11920,7 +11906,7 @@
         <f>_xlfn.XLOOKUP($A22,'2022'!$D$2:$D$13,'2022'!$A$2:$A$13,"x")</f>
         <v>x</v>
       </c>
-      <c r="AO22" s="56" t="str">
+      <c r="AO22" s="37" t="str">
         <f>_xlfn.XLOOKUP($A22,'2023'!$D$2:$D$13,'2023'!$A$2:$A$13,"x")</f>
         <v>x</v>
       </c>
@@ -12092,7 +12078,7 @@
         <f>_xlfn.XLOOKUP($A23,'2022'!$D$2:$D$13,'2022'!$A$2:$A$13,"x")</f>
         <v>0</v>
       </c>
-      <c r="AO23" s="55">
+      <c r="AO23">
         <f>_xlfn.XLOOKUP($A23,'2023'!$D$2:$D$13,'2023'!$A$2:$A$13,"x")</f>
         <v>2</v>
       </c>
@@ -12264,7 +12250,7 @@
         <f>_xlfn.XLOOKUP($A24,'2022'!$D$2:$D$13,'2022'!$A$2:$A$13,"x")</f>
         <v>0</v>
       </c>
-      <c r="AO24" s="56" t="str">
+      <c r="AO24" s="37" t="str">
         <f>_xlfn.XLOOKUP($A24,'2023'!$D$2:$D$13,'2023'!$A$2:$A$13,"x")</f>
         <v>x</v>
       </c>
@@ -12436,7 +12422,7 @@
         <f>_xlfn.XLOOKUP($A25,'2022'!$D$2:$D$13,'2022'!$A$2:$A$13,"x")</f>
         <v>x</v>
       </c>
-      <c r="AO25" s="55">
+      <c r="AO25">
         <f>_xlfn.XLOOKUP($A25,'2023'!$D$2:$D$13,'2023'!$A$2:$A$13,"x")</f>
         <v>6</v>
       </c>
@@ -12607,7 +12593,7 @@
         <v/>
       </c>
       <c r="T29" s="34">
-        <f>SUM(B29:E29)</f>
+        <f t="shared" ref="T29:T43" si="3">SUM(B29:E29)</f>
         <v>16</v>
       </c>
       <c r="U29" s="34"/>
@@ -12635,7 +12621,7 @@
         <v/>
       </c>
       <c r="T30" s="34">
-        <f>SUM(B30:E30)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="U30" s="34"/>
@@ -12663,7 +12649,7 @@
         <v/>
       </c>
       <c r="T31" s="34">
-        <f>SUM(B31:E31)</f>
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
       <c r="U31" s="34"/>
@@ -12691,7 +12677,7 @@
         <v/>
       </c>
       <c r="T32" s="34">
-        <f>SUM(B32:E32)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="U32" s="34"/>
@@ -12719,7 +12705,7 @@
         <v/>
       </c>
       <c r="T33" s="34">
-        <f>SUM(B33:E33)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="U33" s="34"/>
@@ -12747,7 +12733,7 @@
         <v/>
       </c>
       <c r="T34" s="34">
-        <f>SUM(B34:E34)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="U34" s="34"/>
@@ -12775,7 +12761,7 @@
         <v/>
       </c>
       <c r="T35" s="34">
-        <f>SUM(B35:E35)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="U35" s="34"/>
@@ -12803,7 +12789,7 @@
         <v/>
       </c>
       <c r="T36" s="34">
-        <f>SUM(B36:E36)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="U36" s="34"/>
@@ -12831,7 +12817,7 @@
         <v/>
       </c>
       <c r="T37" s="34">
-        <f>SUM(B37:E37)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="U37" s="34"/>
@@ -12859,7 +12845,7 @@
         <v>4</v>
       </c>
       <c r="T38" s="34">
-        <f>SUM(B38:E38)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="U38" s="34"/>
@@ -12887,7 +12873,7 @@
         <v/>
       </c>
       <c r="T39" s="34">
-        <f>SUM(B39:E39)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="U39" s="34"/>
@@ -12915,7 +12901,7 @@
         <v/>
       </c>
       <c r="T40" s="34">
-        <f>SUM(B40:E40)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="U40" s="34"/>
@@ -12943,7 +12929,7 @@
         <v/>
       </c>
       <c r="T41" s="34">
-        <f>SUM(B41:E41)</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="U41" s="34"/>
@@ -12971,7 +12957,7 @@
         <v>6</v>
       </c>
       <c r="T42" s="34">
-        <f>SUM(B42:E42)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="U42" s="34"/>
@@ -12999,7 +12985,7 @@
         <v>3</v>
       </c>
       <c r="T43" s="34">
-        <f>SUM(B43:E43)</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="U43" s="34"/>
@@ -13074,7 +13060,7 @@
         <f>_xlfn.XLOOKUP($A44,'2022'!$D$2:$D$13,'2022'!$E$2:$E$13,"")</f>
         <v>9</v>
       </c>
-      <c r="R44" s="57">
+      <c r="R44" s="29">
         <f>_xlfn.XLOOKUP($A44,'2023'!$D$2:$D$13,'2023'!$E$2:$E$13,"")</f>
         <v>8</v>
       </c>
@@ -13163,7 +13149,7 @@
         <f>_xlfn.XLOOKUP($A45,'2022'!$D$2:$D$13,'2022'!$E$2:$E$13,"")</f>
         <v/>
       </c>
-      <c r="R45" s="56" t="str">
+      <c r="R45" s="37" t="str">
         <f>_xlfn.XLOOKUP($A45,'2023'!$D$2:$D$13,'2023'!$E$2:$E$13,"")</f>
         <v/>
       </c>
@@ -13172,15 +13158,15 @@
         <v/>
       </c>
       <c r="T45" s="34">
-        <f t="shared" ref="T45:T67" si="3">SUM(F45:S45)</f>
+        <f t="shared" ref="T45:T67" si="4">SUM(F45:S45)</f>
         <v>9</v>
       </c>
       <c r="U45" s="34">
-        <f t="shared" ref="U45:U67" si="4">SUM($F$27:$S$27)-SUMIFS($F$27:$S$27,$F45:$S45,"")</f>
+        <f t="shared" ref="U45:U67" si="5">SUM($F$27:$S$27)-SUMIFS($F$27:$S$27,$F45:$S45,"")</f>
         <v>14</v>
       </c>
       <c r="V45" s="34">
-        <f t="shared" ref="V45:V67" si="5">T45/U45</f>
+        <f t="shared" ref="V45:V67" si="6">T45/U45</f>
         <v>0.6428571428571429</v>
       </c>
       <c r="W45" s="34"/>
@@ -13267,7 +13253,7 @@
         <f>_xlfn.XLOOKUP($A46,'2022'!$D$2:$D$13,'2022'!$E$2:$E$13,"")</f>
         <v>10</v>
       </c>
-      <c r="R46" s="57">
+      <c r="R46" s="29">
         <f>_xlfn.XLOOKUP($A46,'2023'!$D$2:$D$13,'2023'!$E$2:$E$13,"")</f>
         <v>7</v>
       </c>
@@ -13276,15 +13262,15 @@
         <v>4</v>
       </c>
       <c r="T46" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>106</v>
       </c>
       <c r="U46" s="29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>189</v>
       </c>
       <c r="V46" s="30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.56084656084656082</v>
       </c>
     </row>
@@ -13356,7 +13342,7 @@
         <f>_xlfn.XLOOKUP($A47,'2022'!$D$2:$D$13,'2022'!$E$2:$E$13,"")</f>
         <v/>
       </c>
-      <c r="R47" s="56" t="str">
+      <c r="R47" s="37" t="str">
         <f>_xlfn.XLOOKUP($A47,'2023'!$D$2:$D$13,'2023'!$E$2:$E$13,"")</f>
         <v/>
       </c>
@@ -13365,15 +13351,15 @@
         <v/>
       </c>
       <c r="T47" s="34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="U47" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="V47" s="34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.5714285714285714</v>
       </c>
       <c r="W47" s="34"/>
@@ -13446,7 +13432,7 @@
         <f>_xlfn.XLOOKUP($A48,'2022'!$D$2:$D$13,'2022'!$E$2:$E$13,"")</f>
         <v>7</v>
       </c>
-      <c r="R48" s="57">
+      <c r="R48" s="29">
         <f>_xlfn.XLOOKUP($A48,'2023'!$D$2:$D$13,'2023'!$E$2:$E$13,"")</f>
         <v>7</v>
       </c>
@@ -13455,15 +13441,15 @@
         <v>8</v>
       </c>
       <c r="T48" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>97</v>
       </c>
       <c r="U48" s="29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>189</v>
       </c>
       <c r="V48" s="30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.51322751322751325</v>
       </c>
     </row>
@@ -13535,7 +13521,7 @@
         <f>_xlfn.XLOOKUP($A49,'2022'!$D$2:$D$13,'2022'!$E$2:$E$13,"")</f>
         <v/>
       </c>
-      <c r="R49" s="56" t="str">
+      <c r="R49" s="37" t="str">
         <f>_xlfn.XLOOKUP($A49,'2023'!$D$2:$D$13,'2023'!$E$2:$E$13,"")</f>
         <v/>
       </c>
@@ -13544,15 +13530,15 @@
         <v/>
       </c>
       <c r="T49" s="34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="U49" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="V49" s="34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.35714285714285715</v>
       </c>
       <c r="W49" s="34"/>
@@ -13625,7 +13611,7 @@
         <f>_xlfn.XLOOKUP($A50,'2022'!$D$2:$D$13,'2022'!$E$2:$E$13,"")</f>
         <v/>
       </c>
-      <c r="R50" s="56" t="str">
+      <c r="R50" s="37" t="str">
         <f>_xlfn.XLOOKUP($A50,'2023'!$D$2:$D$13,'2023'!$E$2:$E$13,"")</f>
         <v/>
       </c>
@@ -13634,15 +13620,15 @@
         <v/>
       </c>
       <c r="T50" s="34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="U50" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="V50" s="34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.2857142857142857</v>
       </c>
       <c r="W50" s="34"/>
@@ -13715,7 +13701,7 @@
         <f>_xlfn.XLOOKUP($A51,'2022'!$D$2:$D$13,'2022'!$E$2:$E$13,"")</f>
         <v>5</v>
       </c>
-      <c r="R51" s="57">
+      <c r="R51" s="29">
         <f>_xlfn.XLOOKUP($A51,'2023'!$D$2:$D$13,'2023'!$E$2:$E$13,"")</f>
         <v>7</v>
       </c>
@@ -13724,15 +13710,15 @@
         <v>11</v>
       </c>
       <c r="T51" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>96</v>
       </c>
       <c r="U51" s="29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>189</v>
       </c>
       <c r="V51" s="30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.50793650793650791</v>
       </c>
     </row>
@@ -13801,7 +13787,7 @@
         <f>_xlfn.XLOOKUP($A52,'2022'!$D$2:$D$13,'2022'!$E$2:$E$13,"")</f>
         <v/>
       </c>
-      <c r="R52" s="56" t="str">
+      <c r="R52" s="37" t="str">
         <f>_xlfn.XLOOKUP($A52,'2023'!$D$2:$D$13,'2023'!$E$2:$E$13,"")</f>
         <v/>
       </c>
@@ -13810,15 +13796,15 @@
         <v/>
       </c>
       <c r="T52" s="34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="U52" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="V52" s="34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.6428571428571429</v>
       </c>
       <c r="W52" s="34"/>
@@ -13887,7 +13873,7 @@
         <f>_xlfn.XLOOKUP($A53,'2022'!$D$2:$D$13,'2022'!$E$2:$E$13,"")</f>
         <v>10</v>
       </c>
-      <c r="R53" s="57">
+      <c r="R53" s="29">
         <f>_xlfn.XLOOKUP($A53,'2023'!$D$2:$D$13,'2023'!$E$2:$E$13,"")</f>
         <v>6</v>
       </c>
@@ -13896,15 +13882,15 @@
         <v>10</v>
       </c>
       <c r="T53" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>95</v>
       </c>
       <c r="U53" s="29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>175</v>
       </c>
       <c r="V53" s="30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.54285714285714282</v>
       </c>
     </row>
@@ -13972,7 +13958,7 @@
         <f>_xlfn.XLOOKUP($A54,'2022'!$D$2:$D$13,'2022'!$E$2:$E$13,"")</f>
         <v>7</v>
       </c>
-      <c r="R54" s="57">
+      <c r="R54" s="29">
         <f>_xlfn.XLOOKUP($A54,'2023'!$D$2:$D$13,'2023'!$E$2:$E$13,"")</f>
         <v>3</v>
       </c>
@@ -13981,15 +13967,15 @@
         <v>2</v>
       </c>
       <c r="T54" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>74</v>
       </c>
       <c r="U54" s="29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>175</v>
       </c>
       <c r="V54" s="30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.42285714285714288</v>
       </c>
     </row>
@@ -14057,7 +14043,7 @@
         <f>_xlfn.XLOOKUP($A55,'2022'!$D$2:$D$13,'2022'!$E$2:$E$13,"")</f>
         <v>7</v>
       </c>
-      <c r="R55" s="57">
+      <c r="R55" s="29">
         <f>_xlfn.XLOOKUP($A55,'2023'!$D$2:$D$13,'2023'!$E$2:$E$13,"")</f>
         <v>6</v>
       </c>
@@ -14066,15 +14052,15 @@
         <v>4</v>
       </c>
       <c r="T55" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>73</v>
       </c>
       <c r="U55" s="29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>175</v>
       </c>
       <c r="V55" s="30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.41714285714285715</v>
       </c>
     </row>
@@ -14142,7 +14128,7 @@
         <f>_xlfn.XLOOKUP($A56,'2022'!$D$2:$D$13,'2022'!$E$2:$E$13,"")</f>
         <v>7</v>
       </c>
-      <c r="R56" s="57">
+      <c r="R56" s="29">
         <f>_xlfn.XLOOKUP($A56,'2023'!$D$2:$D$13,'2023'!$E$2:$E$13,"")</f>
         <v>5</v>
       </c>
@@ -14151,15 +14137,15 @@
         <v>9</v>
       </c>
       <c r="T56" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>78</v>
       </c>
       <c r="U56" s="29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>161</v>
       </c>
       <c r="V56" s="30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.48447204968944102</v>
       </c>
     </row>
@@ -14228,7 +14214,7 @@
         <f>_xlfn.XLOOKUP($A57,'2022'!$D$2:$D$13,'2022'!$E$2:$E$13,"")</f>
         <v/>
       </c>
-      <c r="R57" s="56" t="str">
+      <c r="R57" s="37" t="str">
         <f>_xlfn.XLOOKUP($A57,'2023'!$D$2:$D$13,'2023'!$E$2:$E$13,"")</f>
         <v/>
       </c>
@@ -14237,15 +14223,15 @@
         <v/>
       </c>
       <c r="T57" s="34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="U57" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="V57" s="34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.35714285714285715</v>
       </c>
       <c r="W57" s="34"/>
@@ -14315,7 +14301,7 @@
         <f>_xlfn.XLOOKUP($A58,'2022'!$D$2:$D$13,'2022'!$E$2:$E$13,"")</f>
         <v/>
       </c>
-      <c r="R58" s="56" t="str">
+      <c r="R58" s="37" t="str">
         <f>_xlfn.XLOOKUP($A58,'2023'!$D$2:$D$13,'2023'!$E$2:$E$13,"")</f>
         <v/>
       </c>
@@ -14324,15 +14310,15 @@
         <v/>
       </c>
       <c r="T58" s="34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>23</v>
       </c>
       <c r="U58" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>54</v>
       </c>
       <c r="V58" s="34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.42592592592592593</v>
       </c>
       <c r="W58" s="34"/>
@@ -14402,7 +14388,7 @@
         <f>_xlfn.XLOOKUP($A59,'2022'!$D$2:$D$13,'2022'!$E$2:$E$13,"")</f>
         <v/>
       </c>
-      <c r="R59" s="56" t="str">
+      <c r="R59" s="37" t="str">
         <f>_xlfn.XLOOKUP($A59,'2023'!$D$2:$D$13,'2023'!$E$2:$E$13,"")</f>
         <v/>
       </c>
@@ -14411,15 +14397,15 @@
         <v/>
       </c>
       <c r="T59" s="34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="U59" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
       <c r="V59" s="34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.23076923076923078</v>
       </c>
       <c r="W59" s="34"/>
@@ -14488,7 +14474,7 @@
         <f>_xlfn.XLOOKUP($A60,'2022'!$D$2:$D$13,'2022'!$E$2:$E$13,"")</f>
         <v>5</v>
       </c>
-      <c r="R60" s="57">
+      <c r="R60" s="29">
         <f>_xlfn.XLOOKUP($A60,'2023'!$D$2:$D$13,'2023'!$E$2:$E$13,"")</f>
         <v>7</v>
       </c>
@@ -14497,15 +14483,15 @@
         <v>5</v>
       </c>
       <c r="T60" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>73</v>
       </c>
       <c r="U60" s="29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>147</v>
       </c>
       <c r="V60" s="30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.49659863945578231</v>
       </c>
     </row>
@@ -14573,7 +14559,7 @@
         <f>_xlfn.XLOOKUP($A61,'2022'!$D$2:$D$13,'2022'!$E$2:$E$13,"")</f>
         <v>6</v>
       </c>
-      <c r="R61" s="57">
+      <c r="R61" s="29">
         <f>_xlfn.XLOOKUP($A61,'2023'!$D$2:$D$13,'2023'!$E$2:$E$13,"")</f>
         <v>10</v>
       </c>
@@ -14582,15 +14568,15 @@
         <v>4</v>
       </c>
       <c r="T61" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>71</v>
       </c>
       <c r="U61" s="29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>147</v>
       </c>
       <c r="V61" s="30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.48299319727891155</v>
       </c>
     </row>
@@ -14659,7 +14645,7 @@
         <f>_xlfn.XLOOKUP($A62,'2022'!$D$2:$D$13,'2022'!$E$2:$E$13,"")</f>
         <v/>
       </c>
-      <c r="R62" s="56" t="str">
+      <c r="R62" s="37" t="str">
         <f>_xlfn.XLOOKUP($A62,'2023'!$D$2:$D$13,'2023'!$E$2:$E$13,"")</f>
         <v/>
       </c>
@@ -14668,15 +14654,15 @@
         <v/>
       </c>
       <c r="T62" s="34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="U62" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
       <c r="V62" s="34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.30769230769230771</v>
       </c>
       <c r="W62" s="34"/>
@@ -14746,7 +14732,7 @@
         <f>_xlfn.XLOOKUP($A63,'2022'!$D$2:$D$13,'2022'!$E$2:$E$13,"")</f>
         <v/>
       </c>
-      <c r="R63" s="56" t="str">
+      <c r="R63" s="37" t="str">
         <f>_xlfn.XLOOKUP($A63,'2023'!$D$2:$D$13,'2023'!$E$2:$E$13,"")</f>
         <v/>
       </c>
@@ -14755,15 +14741,15 @@
         <v/>
       </c>
       <c r="T63" s="34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="U63" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
       <c r="V63" s="34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.23076923076923078</v>
       </c>
       <c r="W63" s="34"/>
@@ -14833,7 +14819,7 @@
         <f>_xlfn.XLOOKUP($A64,'2022'!$D$2:$D$13,'2022'!$E$2:$E$13,"")</f>
         <v/>
       </c>
-      <c r="R64" s="56" t="str">
+      <c r="R64" s="37" t="str">
         <f>_xlfn.XLOOKUP($A64,'2023'!$D$2:$D$13,'2023'!$E$2:$E$13,"")</f>
         <v/>
       </c>
@@ -14842,15 +14828,15 @@
         <v/>
       </c>
       <c r="T64" s="34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
       <c r="U64" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>52</v>
       </c>
       <c r="V64" s="34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.53846153846153844</v>
       </c>
       <c r="W64" s="34"/>
@@ -14919,7 +14905,7 @@
         <f>_xlfn.XLOOKUP($A65,'2022'!$D$2:$D$13,'2022'!$E$2:$E$13,"")</f>
         <v>6</v>
       </c>
-      <c r="R65" s="57">
+      <c r="R65" s="29">
         <f>_xlfn.XLOOKUP($A65,'2023'!$D$2:$D$13,'2023'!$E$2:$E$13,"")</f>
         <v>11</v>
       </c>
@@ -14928,15 +14914,15 @@
         <v>8</v>
       </c>
       <c r="T65" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>58</v>
       </c>
       <c r="U65" s="29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>108</v>
       </c>
       <c r="V65" s="30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.53703703703703709</v>
       </c>
     </row>
@@ -15005,7 +14991,7 @@
         <f>_xlfn.XLOOKUP($A66,'2022'!$D$2:$D$13,'2022'!$E$2:$E$13,"")</f>
         <v>5</v>
       </c>
-      <c r="R66" s="56" t="str">
+      <c r="R66" s="37" t="str">
         <f>_xlfn.XLOOKUP($A66,'2023'!$D$2:$D$13,'2023'!$E$2:$E$13,"")</f>
         <v/>
       </c>
@@ -15014,15 +15000,15 @@
         <v/>
       </c>
       <c r="T66" s="34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>23</v>
       </c>
       <c r="U66" s="34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>41</v>
       </c>
       <c r="V66" s="34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.56097560975609762</v>
       </c>
       <c r="W66" s="34"/>
@@ -15091,7 +15077,7 @@
         <f>_xlfn.XLOOKUP($A67,'2022'!$D$2:$D$13,'2022'!$E$2:$E$13,"")</f>
         <v/>
       </c>
-      <c r="R67" s="57">
+      <c r="R67" s="29">
         <f>_xlfn.XLOOKUP($A67,'2023'!$D$2:$D$13,'2023'!$E$2:$E$13,"")</f>
         <v>7</v>
       </c>
@@ -15100,15 +15086,15 @@
         <v>9</v>
       </c>
       <c r="T67" s="29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="U67" s="29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>28</v>
       </c>
       <c r="V67" s="30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.5714285714285714</v>
       </c>
     </row>
@@ -15354,7 +15340,7 @@
       <c r="I2" s="1">
         <v>1401</v>
       </c>
-      <c r="K2" s="40" t="s">
+      <c r="K2" s="41" t="s">
         <v>217</v>
       </c>
     </row>
@@ -15387,8 +15373,8 @@
       <c r="I3" s="1">
         <v>1597</v>
       </c>
-      <c r="K3" s="40"/>
-      <c r="L3" s="38" t="s">
+      <c r="K3" s="41"/>
+      <c r="L3" s="39" t="s">
         <v>217</v>
       </c>
     </row>
@@ -15421,10 +15407,10 @@
       <c r="I4" s="1">
         <v>1324</v>
       </c>
-      <c r="K4" s="37" t="s">
+      <c r="K4" s="38" t="s">
         <v>220</v>
       </c>
-      <c r="L4" s="38"/>
+      <c r="L4" s="39"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -15455,7 +15441,7 @@
       <c r="I5" s="1">
         <v>1364</v>
       </c>
-      <c r="K5" s="37"/>
+      <c r="K5" s="38"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6">
@@ -15513,7 +15499,7 @@
       <c r="I7">
         <v>1311</v>
       </c>
-      <c r="K7" s="37" t="s">
+      <c r="K7" s="38" t="s">
         <v>218</v>
       </c>
     </row>
@@ -15543,8 +15529,8 @@
       <c r="I8">
         <v>1200</v>
       </c>
-      <c r="K8" s="37"/>
-      <c r="L8" s="37" t="s">
+      <c r="K8" s="38"/>
+      <c r="L8" s="38" t="s">
         <v>218</v>
       </c>
     </row>
@@ -15574,13 +15560,13 @@
       <c r="I9">
         <v>985</v>
       </c>
-      <c r="K9" s="38" t="s">
+      <c r="K9" s="39" t="s">
         <v>219</v>
       </c>
-      <c r="L9" s="37"/>
+      <c r="L9" s="38"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K10" s="38"/>
+      <c r="K10" s="39"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L12" s="6" t="s">
@@ -15588,7 +15574,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L13" s="37" t="s">
+      <c r="L13" s="38" t="s">
         <v>220</v>
       </c>
     </row>
@@ -15596,7 +15582,7 @@
       <c r="A14" t="s">
         <v>27</v>
       </c>
-      <c r="L14" s="37"/>
+      <c r="L14" s="38"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -15611,7 +15597,7 @@
       <c r="D15" t="s">
         <v>181</v>
       </c>
-      <c r="L15" s="38" t="s">
+      <c r="L15" s="39" t="s">
         <v>219</v>
       </c>
     </row>
@@ -15628,7 +15614,7 @@
       <c r="D16" t="s">
         <v>186</v>
       </c>
-      <c r="L16" s="38"/>
+      <c r="L16" s="39"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -16077,7 +16063,7 @@
       <c r="I2" s="1">
         <v>1367</v>
       </c>
-      <c r="K2" s="40" t="s">
+      <c r="K2" s="41" t="s">
         <v>245</v>
       </c>
     </row>
@@ -16110,8 +16096,8 @@
       <c r="I3" s="1">
         <v>1409</v>
       </c>
-      <c r="K3" s="40"/>
-      <c r="L3" s="38" t="s">
+      <c r="K3" s="41"/>
+      <c r="L3" s="39" t="s">
         <v>245</v>
       </c>
     </row>
@@ -16144,10 +16130,10 @@
       <c r="I4" s="1">
         <v>1242</v>
       </c>
-      <c r="K4" s="37" t="s">
+      <c r="K4" s="38" t="s">
         <v>247</v>
       </c>
-      <c r="L4" s="38"/>
+      <c r="L4" s="39"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -16178,7 +16164,7 @@
       <c r="I5" s="1">
         <v>1280</v>
       </c>
-      <c r="K5" s="37"/>
+      <c r="K5" s="38"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6">
@@ -16236,7 +16222,7 @@
       <c r="I7">
         <v>1055</v>
       </c>
-      <c r="K7" s="38" t="s">
+      <c r="K7" s="39" t="s">
         <v>246</v>
       </c>
     </row>
@@ -16266,8 +16252,8 @@
       <c r="I8">
         <v>1167</v>
       </c>
-      <c r="K8" s="38"/>
-      <c r="L8" s="37" t="s">
+      <c r="K8" s="39"/>
+      <c r="L8" s="38" t="s">
         <v>246</v>
       </c>
     </row>
@@ -16297,10 +16283,10 @@
       <c r="I9">
         <v>1162</v>
       </c>
-      <c r="K9" s="37" t="s">
+      <c r="K9" s="38" t="s">
         <v>248</v>
       </c>
-      <c r="L9" s="37"/>
+      <c r="L9" s="38"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10">
@@ -16328,7 +16314,7 @@
       <c r="I10">
         <v>1086</v>
       </c>
-      <c r="K10" s="37"/>
+      <c r="K10" s="38"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11">
@@ -16363,7 +16349,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L13" s="38" t="s">
+      <c r="L13" s="39" t="s">
         <v>247</v>
       </c>
     </row>
@@ -16371,13 +16357,13 @@
       <c r="A14" t="s">
         <v>27</v>
       </c>
-      <c r="L14" s="38"/>
+      <c r="L14" s="39"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>174</v>
       </c>
-      <c r="L15" s="37" t="s">
+      <c r="L15" s="38" t="s">
         <v>248</v>
       </c>
     </row>
@@ -16385,7 +16371,7 @@
       <c r="A16" t="s">
         <v>28</v>
       </c>
-      <c r="L16" s="37"/>
+      <c r="L16" s="38"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -16500,7 +16486,7 @@
       <c r="I2" s="1">
         <v>1830.14</v>
       </c>
-      <c r="K2" s="37" t="s">
+      <c r="K2" s="38" t="s">
         <v>13</v>
       </c>
     </row>
@@ -16533,8 +16519,8 @@
       <c r="I3" s="1">
         <v>1705.42</v>
       </c>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37" t="s">
+      <c r="K3" s="38"/>
+      <c r="L3" s="38" t="s">
         <v>260</v>
       </c>
     </row>
@@ -16567,10 +16553,10 @@
       <c r="I4" s="1">
         <v>1633.02</v>
       </c>
-      <c r="K4" s="38" t="s">
+      <c r="K4" s="39" t="s">
         <v>260</v>
       </c>
-      <c r="L4" s="37"/>
+      <c r="L4" s="38"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -16601,7 +16587,7 @@
       <c r="I5" s="1">
         <v>1611.72</v>
       </c>
-      <c r="K5" s="38"/>
+      <c r="K5" s="39"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6">
@@ -16659,7 +16645,7 @@
       <c r="I7">
         <v>1547.34</v>
       </c>
-      <c r="K7" s="38" t="s">
+      <c r="K7" s="39" t="s">
         <v>259</v>
       </c>
     </row>
@@ -16689,8 +16675,8 @@
       <c r="I8">
         <v>1316.64</v>
       </c>
-      <c r="K8" s="38"/>
-      <c r="L8" s="38" t="s">
+      <c r="K8" s="39"/>
+      <c r="L8" s="39" t="s">
         <v>259</v>
       </c>
     </row>
@@ -16720,13 +16706,13 @@
       <c r="I9">
         <v>1320.34</v>
       </c>
-      <c r="K9" s="37" t="s">
+      <c r="K9" s="38" t="s">
         <v>261</v>
       </c>
-      <c r="L9" s="38"/>
+      <c r="L9" s="39"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K10" s="37"/>
+      <c r="K10" s="38"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L12" s="6" t="s">
@@ -16734,7 +16720,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L13" s="38" t="s">
+      <c r="L13" s="39" t="s">
         <v>13</v>
       </c>
     </row>
@@ -16745,7 +16731,7 @@
       <c r="B14" s="7" t="s">
         <v>268</v>
       </c>
-      <c r="L14" s="38"/>
+      <c r="L14" s="39"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -16754,7 +16740,7 @@
       <c r="B15" s="7" t="s">
         <v>269</v>
       </c>
-      <c r="L15" s="37" t="s">
+      <c r="L15" s="38" t="s">
         <v>261</v>
       </c>
     </row>
@@ -16765,7 +16751,7 @@
       <c r="B16" s="7" t="s">
         <v>270</v>
       </c>
-      <c r="L16" s="37"/>
+      <c r="L16" s="38"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -16891,7 +16877,7 @@
       <c r="I2" s="1">
         <v>1636</v>
       </c>
-      <c r="K2" s="40" t="s">
+      <c r="K2" s="41" t="s">
         <v>7</v>
       </c>
     </row>
@@ -16924,8 +16910,8 @@
       <c r="I3" s="1">
         <v>1450</v>
       </c>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40" t="s">
+      <c r="K3" s="41"/>
+      <c r="L3" s="41" t="s">
         <v>7</v>
       </c>
     </row>
@@ -16958,10 +16944,10 @@
       <c r="I4" s="1">
         <v>1333</v>
       </c>
-      <c r="K4" s="37" t="s">
+      <c r="K4" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="40"/>
+      <c r="L4" s="41"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -16992,7 +16978,7 @@
       <c r="I5" s="1">
         <v>1558</v>
       </c>
-      <c r="K5" s="37"/>
+      <c r="K5" s="38"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6">
@@ -17050,7 +17036,7 @@
       <c r="I7">
         <v>1141</v>
       </c>
-      <c r="K7" s="37" t="s">
+      <c r="K7" s="38" t="s">
         <v>13</v>
       </c>
     </row>
@@ -17080,8 +17066,8 @@
       <c r="I8">
         <v>1174</v>
       </c>
-      <c r="K8" s="37"/>
-      <c r="L8" s="37" t="s">
+      <c r="K8" s="38"/>
+      <c r="L8" s="38" t="s">
         <v>9</v>
       </c>
     </row>
@@ -17111,13 +17097,13 @@
       <c r="I9">
         <v>1344</v>
       </c>
-      <c r="K9" s="38" t="s">
+      <c r="K9" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="L9" s="37"/>
+      <c r="L9" s="38"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="K10" s="38"/>
+      <c r="K10" s="39"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L12" s="6" t="s">
@@ -17125,7 +17111,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L13" s="37" t="s">
+      <c r="L13" s="38" t="s">
         <v>11</v>
       </c>
     </row>
@@ -17136,7 +17122,7 @@
       <c r="B14" t="s">
         <v>34</v>
       </c>
-      <c r="L14" s="37"/>
+      <c r="L14" s="38"/>
       <c r="M14" t="s">
         <v>11</v>
       </c>
@@ -17145,7 +17131,7 @@
       <c r="A15" t="s">
         <v>26</v>
       </c>
-      <c r="L15" s="37" t="s">
+      <c r="L15" s="38" t="s">
         <v>13</v>
       </c>
     </row>
@@ -17153,7 +17139,7 @@
       <c r="A16" t="s">
         <v>28</v>
       </c>
-      <c r="L16" s="37"/>
+      <c r="L16" s="38"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -17273,7 +17259,7 @@
       <c r="I2" s="1">
         <v>1511</v>
       </c>
-      <c r="K2" s="37" t="s">
+      <c r="K2" s="38" t="s">
         <v>9</v>
       </c>
     </row>
@@ -17306,8 +17292,8 @@
       <c r="I3" s="1">
         <v>1402</v>
       </c>
-      <c r="K3" s="37"/>
-      <c r="L3" s="38" t="s">
+      <c r="K3" s="38"/>
+      <c r="L3" s="39" t="s">
         <v>35</v>
       </c>
     </row>
@@ -17340,10 +17326,10 @@
       <c r="I4" s="1">
         <v>1297</v>
       </c>
-      <c r="K4" s="38" t="s">
+      <c r="K4" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="L4" s="38"/>
+      <c r="L4" s="39"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -17374,7 +17360,7 @@
       <c r="I5" s="1">
         <v>1398</v>
       </c>
-      <c r="K5" s="38"/>
+      <c r="K5" s="39"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6">
@@ -17432,7 +17418,7 @@
       <c r="I7">
         <v>1269</v>
       </c>
-      <c r="K7" s="38" t="s">
+      <c r="K7" s="39" t="s">
         <v>36</v>
       </c>
     </row>
@@ -17462,8 +17448,8 @@
       <c r="I8">
         <v>1254</v>
       </c>
-      <c r="K8" s="38"/>
-      <c r="L8" s="37" t="s">
+      <c r="K8" s="39"/>
+      <c r="L8" s="38" t="s">
         <v>9</v>
       </c>
     </row>
@@ -17493,10 +17479,10 @@
       <c r="I9">
         <v>1351</v>
       </c>
-      <c r="K9" s="37" t="s">
+      <c r="K9" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="L9" s="37"/>
+      <c r="L9" s="38"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10">
@@ -17524,7 +17510,7 @@
       <c r="I10">
         <v>1294</v>
       </c>
-      <c r="K10" s="37"/>
+      <c r="K10" s="38"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11">
@@ -17559,7 +17545,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L13" s="38" t="s">
+      <c r="L13" s="39" t="s">
         <v>9</v>
       </c>
     </row>
@@ -17570,7 +17556,7 @@
       <c r="B14" t="s">
         <v>34</v>
       </c>
-      <c r="L14" s="38"/>
+      <c r="L14" s="39"/>
       <c r="M14" t="s">
         <v>9</v>
       </c>
@@ -17588,7 +17574,7 @@
       <c r="F15" s="15">
         <v>120</v>
       </c>
-      <c r="L15" s="37" t="s">
+      <c r="L15" s="38" t="s">
         <v>37</v>
       </c>
     </row>
@@ -17603,7 +17589,7 @@
       <c r="F16" s="15">
         <v>60</v>
       </c>
-      <c r="L16" s="37"/>
+      <c r="L16" s="38"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -17731,7 +17717,7 @@
       <c r="I2" s="1">
         <v>1844.5</v>
       </c>
-      <c r="K2" s="37" t="str">
+      <c r="K2" s="38" t="str">
         <f>C2</f>
         <v>#Hashtags</v>
       </c>
@@ -17765,8 +17751,8 @@
       <c r="I3" s="1">
         <v>2096.08</v>
       </c>
-      <c r="K3" s="37"/>
-      <c r="L3" s="38" t="s">
+      <c r="K3" s="38"/>
+      <c r="L3" s="39" t="s">
         <v>50</v>
       </c>
     </row>
@@ -17799,11 +17785,11 @@
       <c r="I4" s="1">
         <v>1811.46</v>
       </c>
-      <c r="K4" s="38" t="str">
+      <c r="K4" s="39" t="str">
         <f>C5</f>
         <v>Bologna Ponies</v>
       </c>
-      <c r="L4" s="38"/>
+      <c r="L4" s="39"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -17834,7 +17820,7 @@
       <c r="I5" s="1">
         <v>2048.5</v>
       </c>
-      <c r="K5" s="38"/>
+      <c r="K5" s="39"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6">
@@ -17892,7 +17878,7 @@
       <c r="I7">
         <v>1774.8</v>
       </c>
-      <c r="K7" s="38" t="str">
+      <c r="K7" s="39" t="str">
         <f>C3</f>
         <v>The Timmies</v>
       </c>
@@ -17923,8 +17909,8 @@
       <c r="I8">
         <v>1793.28</v>
       </c>
-      <c r="K8" s="38"/>
-      <c r="L8" s="37" t="s">
+      <c r="K8" s="39"/>
+      <c r="L8" s="38" t="s">
         <v>51</v>
       </c>
     </row>
@@ -17954,11 +17940,11 @@
       <c r="I9">
         <v>1922.56</v>
       </c>
-      <c r="K9" s="37" t="str">
+      <c r="K9" s="38" t="str">
         <f>C4</f>
         <v>The dago</v>
       </c>
-      <c r="L9" s="37"/>
+      <c r="L9" s="38"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10">
@@ -17986,7 +17972,7 @@
       <c r="I10">
         <v>1882.62</v>
       </c>
-      <c r="K10" s="37"/>
+      <c r="K10" s="38"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11">
@@ -18021,7 +18007,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L13" s="38" t="s">
+      <c r="L13" s="39" t="s">
         <v>7</v>
       </c>
     </row>
@@ -18032,7 +18018,7 @@
       <c r="B14" t="s">
         <v>34</v>
       </c>
-      <c r="L14" s="38"/>
+      <c r="L14" s="39"/>
       <c r="M14" t="s">
         <v>7</v>
       </c>
@@ -18050,7 +18036,7 @@
       <c r="F15" s="16">
         <v>120</v>
       </c>
-      <c r="L15" s="37" t="s">
+      <c r="L15" s="38" t="s">
         <v>52</v>
       </c>
     </row>
@@ -18064,7 +18050,7 @@
       <c r="F16" s="16">
         <v>60</v>
       </c>
-      <c r="L16" s="37"/>
+      <c r="L16" s="38"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -18215,7 +18201,7 @@
       <c r="J3" s="1">
         <v>1596.84</v>
       </c>
-      <c r="L3" s="38" t="s">
+      <c r="L3" s="39" t="s">
         <v>79</v>
       </c>
     </row>
@@ -18251,7 +18237,7 @@
       <c r="J4" s="1">
         <v>1481.24</v>
       </c>
-      <c r="L4" s="45"/>
+      <c r="L4" s="42"/>
       <c r="M4" s="10"/>
     </row>
     <row r="5" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -18286,7 +18272,7 @@
       <c r="J5" s="1">
         <v>1728.66</v>
       </c>
-      <c r="L5" s="39" t="s">
+      <c r="L5" s="40" t="s">
         <v>80</v>
       </c>
       <c r="N5" s="14"/>
@@ -18323,8 +18309,8 @@
       <c r="J6" s="1">
         <v>1635.62</v>
       </c>
-      <c r="L6" s="39"/>
-      <c r="N6" s="41" t="s">
+      <c r="L6" s="40"/>
+      <c r="N6" s="44" t="s">
         <v>79</v>
       </c>
     </row>
@@ -18357,7 +18343,7 @@
       <c r="J7">
         <v>1508.98</v>
       </c>
-      <c r="N7" s="46"/>
+      <c r="N7" s="45"/>
       <c r="O7" s="10"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -18390,7 +18376,7 @@
       <c r="J8" s="10">
         <v>1388.18</v>
       </c>
-      <c r="N8" s="42" t="s">
+      <c r="N8" s="43" t="s">
         <v>51</v>
       </c>
       <c r="P8" s="14"/>
@@ -18399,10 +18385,10 @@
       <c r="A9" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="L9" s="38" t="s">
+      <c r="L9" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="N9" s="42"/>
+      <c r="N9" s="43"/>
       <c r="P9" s="14"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -18436,7 +18422,7 @@
       <c r="J10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="L10" s="45"/>
+      <c r="L10" s="42"/>
       <c r="M10" s="10"/>
       <c r="N10" s="14"/>
       <c r="P10" s="14"/>
@@ -18473,7 +18459,7 @@
       <c r="J11" s="1">
         <v>1673.14</v>
       </c>
-      <c r="L11" s="37" t="s">
+      <c r="L11" s="38" t="s">
         <v>61</v>
       </c>
       <c r="P11" s="14"/>
@@ -18510,8 +18496,8 @@
       <c r="J12" s="1">
         <v>1615.32</v>
       </c>
-      <c r="L12" s="37"/>
-      <c r="P12" s="42" t="s">
+      <c r="L12" s="38"/>
+      <c r="P12" s="43" t="s">
         <v>51</v>
       </c>
     </row>
@@ -18544,7 +18530,7 @@
       <c r="J13">
         <v>1539.26</v>
       </c>
-      <c r="P13" s="43"/>
+      <c r="P13" s="47"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B14">
@@ -18575,7 +18561,7 @@
       <c r="J14">
         <v>1336.24</v>
       </c>
-      <c r="P14" s="41" t="s">
+      <c r="P14" s="44" t="s">
         <v>70</v>
       </c>
     </row>
@@ -18608,10 +18594,10 @@
       <c r="J15">
         <v>1368.88</v>
       </c>
-      <c r="L15" s="37" t="s">
+      <c r="L15" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="P15" s="41"/>
+      <c r="P15" s="44"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B16">
@@ -18642,12 +18628,12 @@
       <c r="J16">
         <v>1513.46</v>
       </c>
-      <c r="L16" s="44"/>
+      <c r="L16" s="46"/>
       <c r="M16" s="10"/>
       <c r="P16" s="14"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L17" s="38" t="s">
+      <c r="L17" s="39" t="s">
         <v>70</v>
       </c>
       <c r="N17" s="14"/>
@@ -18655,20 +18641,20 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H18" s="4"/>
-      <c r="L18" s="38"/>
-      <c r="N18" s="41" t="s">
+      <c r="L18" s="39"/>
+      <c r="N18" s="44" t="s">
         <v>70</v>
       </c>
       <c r="P18" s="14"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H19" s="4"/>
-      <c r="N19" s="46"/>
+      <c r="N19" s="45"/>
       <c r="O19" s="10"/>
       <c r="P19" s="14"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="N20" s="42" t="s">
+      <c r="N20" s="43" t="s">
         <v>60</v>
       </c>
     </row>
@@ -18682,10 +18668,10 @@
       <c r="F21" s="16">
         <v>120</v>
       </c>
-      <c r="L21" s="38" t="s">
+      <c r="L21" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="N21" s="42"/>
+      <c r="N21" s="43"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -18700,7 +18686,7 @@
       <c r="F22" s="16">
         <v>60</v>
       </c>
-      <c r="L22" s="45"/>
+      <c r="L22" s="42"/>
       <c r="M22" s="10"/>
       <c r="N22" s="14"/>
     </row>
@@ -18714,7 +18700,7 @@
       <c r="F23" s="16">
         <v>20</v>
       </c>
-      <c r="L23" s="37" t="s">
+      <c r="L23" s="38" t="s">
         <v>80</v>
       </c>
     </row>
@@ -18722,7 +18708,7 @@
       <c r="A24" t="s">
         <v>28</v>
       </c>
-      <c r="L24" s="37"/>
+      <c r="L24" s="38"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -18736,7 +18722,7 @@
       <c r="A26" t="s">
         <v>30</v>
       </c>
-      <c r="P26" s="37" t="s">
+      <c r="P26" s="38" t="s">
         <v>79</v>
       </c>
     </row>
@@ -18744,13 +18730,13 @@
       <c r="A27" t="s">
         <v>83</v>
       </c>
-      <c r="P27" s="44"/>
+      <c r="P27" s="46"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>32</v>
       </c>
-      <c r="P28" s="38" t="s">
+      <c r="P28" s="39" t="s">
         <v>60</v>
       </c>
     </row>
@@ -18758,13 +18744,19 @@
       <c r="A29" t="s">
         <v>49</v>
       </c>
-      <c r="P29" s="38"/>
+      <c r="P29" s="39"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C11:J16">
     <sortCondition descending="1" ref="H11:H16"/>
   </sortState>
   <mergeCells count="16">
+    <mergeCell ref="P14:P15"/>
+    <mergeCell ref="P12:P13"/>
+    <mergeCell ref="P28:P29"/>
+    <mergeCell ref="P26:P27"/>
+    <mergeCell ref="L23:L24"/>
+    <mergeCell ref="L21:L22"/>
     <mergeCell ref="L3:L4"/>
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="N8:N9"/>
@@ -18775,12 +18767,6 @@
     <mergeCell ref="L11:L12"/>
     <mergeCell ref="L15:L16"/>
     <mergeCell ref="L17:L18"/>
-    <mergeCell ref="P14:P15"/>
-    <mergeCell ref="P12:P13"/>
-    <mergeCell ref="P28:P29"/>
-    <mergeCell ref="P26:P27"/>
-    <mergeCell ref="L23:L24"/>
-    <mergeCell ref="L21:L22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18886,7 +18872,7 @@
       <c r="J3" s="1">
         <v>1732.22</v>
       </c>
-      <c r="L3" s="38" t="s">
+      <c r="L3" s="39" t="s">
         <v>86</v>
       </c>
     </row>
@@ -18922,7 +18908,7 @@
       <c r="J4" s="1">
         <v>1639.06</v>
       </c>
-      <c r="L4" s="45"/>
+      <c r="L4" s="42"/>
       <c r="M4" s="10"/>
     </row>
     <row r="5" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -18957,7 +18943,7 @@
       <c r="J5" s="1">
         <v>1533.2</v>
       </c>
-      <c r="L5" s="39" t="s">
+      <c r="L5" s="40" t="s">
         <v>80</v>
       </c>
       <c r="N5" s="14"/>
@@ -18994,8 +18980,8 @@
       <c r="J6" s="1">
         <v>1643.26</v>
       </c>
-      <c r="L6" s="39"/>
-      <c r="N6" s="41" t="s">
+      <c r="L6" s="40"/>
+      <c r="N6" s="44" t="s">
         <v>86</v>
       </c>
     </row>
@@ -19028,7 +19014,7 @@
       <c r="J7">
         <v>1588.24</v>
       </c>
-      <c r="N7" s="46"/>
+      <c r="N7" s="45"/>
       <c r="O7" s="10"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -19061,7 +19047,7 @@
       <c r="J8" s="10">
         <v>1475.86</v>
       </c>
-      <c r="N8" s="42" t="s">
+      <c r="N8" s="43" t="s">
         <v>89</v>
       </c>
       <c r="P8" s="14"/>
@@ -19070,10 +19056,10 @@
       <c r="A9" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="L9" s="37" t="s">
+      <c r="L9" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="N9" s="42"/>
+      <c r="N9" s="43"/>
       <c r="P9" s="14"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -19107,7 +19093,7 @@
       <c r="J10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="L10" s="44"/>
+      <c r="L10" s="46"/>
       <c r="M10" s="10"/>
       <c r="N10" s="14"/>
       <c r="P10" s="14"/>
@@ -19144,7 +19130,7 @@
       <c r="J11" s="1">
         <v>1625.18</v>
       </c>
-      <c r="L11" s="38" t="s">
+      <c r="L11" s="39" t="s">
         <v>89</v>
       </c>
       <c r="P11" s="14"/>
@@ -19181,8 +19167,8 @@
       <c r="J12" s="1">
         <v>1578.96</v>
       </c>
-      <c r="L12" s="38"/>
-      <c r="P12" s="42" t="s">
+      <c r="L12" s="39"/>
+      <c r="P12" s="43" t="s">
         <v>86</v>
       </c>
     </row>
@@ -19215,7 +19201,7 @@
       <c r="J13">
         <v>1497.04</v>
       </c>
-      <c r="P13" s="43"/>
+      <c r="P13" s="47"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B14">
@@ -19246,7 +19232,7 @@
       <c r="J14">
         <v>1303.76</v>
       </c>
-      <c r="P14" s="41" t="s">
+      <c r="P14" s="44" t="s">
         <v>88</v>
       </c>
     </row>
@@ -19279,10 +19265,10 @@
       <c r="J15">
         <v>1504.64</v>
       </c>
-      <c r="L15" s="37" t="s">
+      <c r="L15" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="P15" s="41"/>
+      <c r="P15" s="44"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B16">
@@ -19313,12 +19299,12 @@
       <c r="J16">
         <v>1382.22</v>
       </c>
-      <c r="L16" s="44"/>
+      <c r="L16" s="46"/>
       <c r="M16" s="10"/>
       <c r="P16" s="14"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="L17" s="38" t="s">
+      <c r="L17" s="39" t="s">
         <v>72</v>
       </c>
       <c r="N17" s="14"/>
@@ -19326,20 +19312,20 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H18" s="4"/>
-      <c r="L18" s="38"/>
-      <c r="N18" s="41" t="s">
+      <c r="L18" s="39"/>
+      <c r="N18" s="44" t="s">
         <v>72</v>
       </c>
       <c r="P18" s="14"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H19" s="4"/>
-      <c r="N19" s="46"/>
+      <c r="N19" s="45"/>
       <c r="O19" s="10"/>
       <c r="P19" s="14"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="N20" s="42" t="s">
+      <c r="N20" s="43" t="s">
         <v>88</v>
       </c>
     </row>
@@ -19353,10 +19339,10 @@
       <c r="F21" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="L21" s="38" t="s">
+      <c r="L21" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="N21" s="42"/>
+      <c r="N21" s="43"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -19371,7 +19357,7 @@
       <c r="F22" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="L22" s="45"/>
+      <c r="L22" s="42"/>
       <c r="M22" s="10"/>
       <c r="N22" s="14"/>
     </row>
@@ -19385,7 +19371,7 @@
       <c r="F23" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="L23" s="37" t="s">
+      <c r="L23" s="38" t="s">
         <v>80</v>
       </c>
     </row>
@@ -19397,7 +19383,7 @@
         <v>112</v>
       </c>
       <c r="F24" s="16"/>
-      <c r="L24" s="37"/>
+      <c r="L24" s="38"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -19412,7 +19398,7 @@
       <c r="A26" t="s">
         <v>30</v>
       </c>
-      <c r="P26" s="38" t="s">
+      <c r="P26" s="39" t="s">
         <v>89</v>
       </c>
     </row>
@@ -19420,13 +19406,13 @@
       <c r="A27" t="s">
         <v>83</v>
       </c>
-      <c r="P27" s="45"/>
+      <c r="P27" s="42"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>32</v>
       </c>
-      <c r="P28" s="37" t="s">
+      <c r="P28" s="38" t="s">
         <v>72</v>
       </c>
     </row>
@@ -19434,18 +19420,13 @@
       <c r="A29" t="s">
         <v>49</v>
       </c>
-      <c r="P29" s="37"/>
+      <c r="P29" s="38"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C11:J16">
     <sortCondition descending="1" ref="H11:H16"/>
   </sortState>
   <mergeCells count="16">
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="L9:L10"/>
     <mergeCell ref="L23:L24"/>
     <mergeCell ref="P26:P27"/>
     <mergeCell ref="P28:P29"/>
@@ -19457,6 +19438,11 @@
     <mergeCell ref="N20:N21"/>
     <mergeCell ref="L21:L22"/>
     <mergeCell ref="L11:L12"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="L9:L10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update history to include 2024 champs
</commit_message>
<xml_diff>
--- a/TeamFriends_History.xlsx
+++ b/TeamFriends_History.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Sites\TeamFriendsFantasy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F652E3A2-3019-4B9A-8063-7AA110B07CF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA3B8299-1570-4514-B1C2-DDC1ACA39844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="677" activeTab="17" xr2:uid="{960D14EB-F112-4860-840A-1E6B67EAFFB3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="677" activeTab="18" xr2:uid="{960D14EB-F112-4860-840A-1E6B67EAFFB3}"/>
   </bookViews>
   <sheets>
     <sheet name="2005" sheetId="16" r:id="rId1"/>
@@ -1175,22 +1175,22 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2343,7 +2343,7 @@
       <c r="J4" s="1">
         <v>1595.7</v>
       </c>
-      <c r="L4" s="46"/>
+      <c r="L4" s="42"/>
       <c r="M4" s="10"/>
     </row>
     <row r="5" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2416,7 +2416,7 @@
         <v>1622.42</v>
       </c>
       <c r="L6" s="40"/>
-      <c r="N6" s="42" t="s">
+      <c r="N6" s="44" t="s">
         <v>97</v>
       </c>
     </row>
@@ -2449,7 +2449,7 @@
       <c r="J7">
         <v>1329.76</v>
       </c>
-      <c r="N7" s="47"/>
+      <c r="N7" s="45"/>
       <c r="O7" s="10"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -2528,7 +2528,7 @@
       <c r="J10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="L10" s="46"/>
+      <c r="L10" s="42"/>
       <c r="M10" s="10"/>
       <c r="N10" s="14"/>
       <c r="P10" s="14"/>
@@ -2636,7 +2636,7 @@
       <c r="J13">
         <v>1604.78</v>
       </c>
-      <c r="P13" s="44"/>
+      <c r="P13" s="47"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B14">
@@ -2667,7 +2667,7 @@
       <c r="J14">
         <v>1563.12</v>
       </c>
-      <c r="P14" s="42" t="s">
+      <c r="P14" s="44" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2703,7 +2703,7 @@
       <c r="L15" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="P15" s="42"/>
+      <c r="P15" s="44"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B16">
@@ -2734,7 +2734,7 @@
       <c r="J16">
         <v>1463.6</v>
       </c>
-      <c r="L16" s="46"/>
+      <c r="L16" s="42"/>
       <c r="M16" s="10"/>
       <c r="P16" s="14"/>
     </row>
@@ -2748,14 +2748,14 @@
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H18" s="4"/>
       <c r="L18" s="38"/>
-      <c r="N18" s="42" t="s">
+      <c r="N18" s="44" t="s">
         <v>73</v>
       </c>
       <c r="P18" s="14"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H19" s="4"/>
-      <c r="N19" s="47"/>
+      <c r="N19" s="45"/>
       <c r="O19" s="10"/>
       <c r="P19" s="14"/>
     </row>
@@ -2792,7 +2792,7 @@
       <c r="F22" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="L22" s="46"/>
+      <c r="L22" s="42"/>
       <c r="M22" s="10"/>
       <c r="N22" s="14"/>
     </row>
@@ -2843,7 +2843,7 @@
       <c r="A27" t="s">
         <v>83</v>
       </c>
-      <c r="P27" s="45"/>
+      <c r="P27" s="46"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -2864,11 +2864,6 @@
     <sortCondition descending="1" ref="H3:H8"/>
   </sortState>
   <mergeCells count="16">
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="L9:L10"/>
     <mergeCell ref="L23:L24"/>
     <mergeCell ref="P26:P27"/>
     <mergeCell ref="P28:P29"/>
@@ -2880,6 +2875,11 @@
     <mergeCell ref="N20:N21"/>
     <mergeCell ref="L21:L22"/>
     <mergeCell ref="L11:L12"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="L9:L10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3021,7 +3021,7 @@
       <c r="J4" s="1">
         <v>1541.96</v>
       </c>
-      <c r="L4" s="46"/>
+      <c r="L4" s="42"/>
       <c r="M4" s="10"/>
     </row>
     <row r="5" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3124,7 +3124,7 @@
       <c r="J7">
         <v>1396.52</v>
       </c>
-      <c r="N7" s="44"/>
+      <c r="N7" s="47"/>
       <c r="O7" s="10"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -3157,7 +3157,7 @@
       <c r="J8" s="10">
         <v>1071.8599999999999</v>
       </c>
-      <c r="N8" s="42" t="s">
+      <c r="N8" s="44" t="s">
         <v>60</v>
       </c>
       <c r="P8" s="14"/>
@@ -3169,7 +3169,7 @@
       <c r="L9" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="N9" s="42"/>
+      <c r="N9" s="44"/>
       <c r="P9" s="14"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -3203,7 +3203,7 @@
       <c r="J10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="L10" s="45"/>
+      <c r="L10" s="46"/>
       <c r="M10" s="10"/>
       <c r="N10" s="14"/>
       <c r="P10" s="14"/>
@@ -3314,7 +3314,7 @@
       <c r="J13" s="1">
         <v>1559.22</v>
       </c>
-      <c r="P13" s="44"/>
+      <c r="P13" s="47"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B14">
@@ -3345,7 +3345,7 @@
       <c r="J14">
         <v>1534.62</v>
       </c>
-      <c r="P14" s="42" t="s">
+      <c r="P14" s="44" t="s">
         <v>115</v>
       </c>
     </row>
@@ -3381,7 +3381,7 @@
       <c r="L15" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="P15" s="42"/>
+      <c r="P15" s="44"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B16">
@@ -3412,7 +3412,7 @@
       <c r="J16">
         <v>1163.0999999999999</v>
       </c>
-      <c r="L16" s="46"/>
+      <c r="L16" s="42"/>
       <c r="M16" s="10"/>
       <c r="P16" s="14"/>
     </row>
@@ -3426,14 +3426,14 @@
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H18" s="4"/>
       <c r="L18" s="38"/>
-      <c r="N18" s="42" t="s">
+      <c r="N18" s="44" t="s">
         <v>73</v>
       </c>
       <c r="P18" s="14"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H19" s="4"/>
-      <c r="N19" s="47"/>
+      <c r="N19" s="45"/>
       <c r="O19" s="10"/>
       <c r="P19" s="14"/>
     </row>
@@ -3470,7 +3470,7 @@
       <c r="F22" s="16">
         <v>100</v>
       </c>
-      <c r="L22" s="46"/>
+      <c r="L22" s="42"/>
       <c r="M22" s="10"/>
       <c r="N22" s="14"/>
     </row>
@@ -3533,7 +3533,7 @@
       <c r="A27" t="s">
         <v>83</v>
       </c>
-      <c r="P27" s="45"/>
+      <c r="P27" s="46"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -3554,11 +3554,6 @@
     <sortCondition descending="1" ref="H11:H16"/>
   </sortState>
   <mergeCells count="16">
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="L9:L10"/>
     <mergeCell ref="L23:L24"/>
     <mergeCell ref="P26:P27"/>
     <mergeCell ref="P28:P29"/>
@@ -3570,6 +3565,11 @@
     <mergeCell ref="N20:N21"/>
     <mergeCell ref="L21:L22"/>
     <mergeCell ref="L11:L12"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="L9:L10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3711,7 +3711,7 @@
       <c r="J4" s="1">
         <v>1746.74</v>
       </c>
-      <c r="L4" s="46"/>
+      <c r="L4" s="42"/>
       <c r="M4" s="10"/>
     </row>
     <row r="5" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3778,7 +3778,7 @@
         <v>1608.62</v>
       </c>
       <c r="L6" s="40"/>
-      <c r="N6" s="42" t="s">
+      <c r="N6" s="44" t="s">
         <v>123</v>
       </c>
     </row>
@@ -3811,7 +3811,7 @@
       <c r="J7">
         <v>1608.1</v>
       </c>
-      <c r="N7" s="47"/>
+      <c r="N7" s="45"/>
       <c r="O7" s="10"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -3890,7 +3890,7 @@
       <c r="J10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="L10" s="46"/>
+      <c r="L10" s="42"/>
       <c r="M10" s="10"/>
       <c r="N10" s="14"/>
       <c r="P10" s="14"/>
@@ -3965,7 +3965,7 @@
         <v>1666.54</v>
       </c>
       <c r="L12" s="38"/>
-      <c r="P12" s="42" t="s">
+      <c r="P12" s="44" t="s">
         <v>116</v>
       </c>
     </row>
@@ -4001,7 +4001,7 @@
       <c r="J13" s="1">
         <v>1770.32</v>
       </c>
-      <c r="P13" s="47"/>
+      <c r="P13" s="45"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -4102,7 +4102,7 @@
       <c r="J16">
         <v>1310.1400000000001</v>
       </c>
-      <c r="L16" s="45"/>
+      <c r="L16" s="46"/>
       <c r="M16" s="10"/>
       <c r="P16" s="14"/>
     </row>
@@ -4123,12 +4123,12 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H19" s="4"/>
-      <c r="N19" s="44"/>
+      <c r="N19" s="47"/>
       <c r="O19" s="10"/>
       <c r="P19" s="14"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="N20" s="42" t="s">
+      <c r="N20" s="44" t="s">
         <v>60</v>
       </c>
     </row>
@@ -4145,7 +4145,7 @@
       <c r="L21" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="N21" s="42"/>
+      <c r="N21" s="44"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -4160,7 +4160,7 @@
       <c r="F22" s="16">
         <v>100</v>
       </c>
-      <c r="L22" s="46"/>
+      <c r="L22" s="42"/>
       <c r="M22" s="10"/>
       <c r="N22" s="14"/>
     </row>
@@ -4223,7 +4223,7 @@
       <c r="A27" t="s">
         <v>83</v>
       </c>
-      <c r="P27" s="46"/>
+      <c r="P27" s="42"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -4244,11 +4244,6 @@
     <sortCondition descending="1" ref="H11:H16"/>
   </sortState>
   <mergeCells count="16">
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="L9:L10"/>
     <mergeCell ref="L23:L24"/>
     <mergeCell ref="P26:P27"/>
     <mergeCell ref="P28:P29"/>
@@ -4260,6 +4255,11 @@
     <mergeCell ref="N20:N21"/>
     <mergeCell ref="L21:L22"/>
     <mergeCell ref="L11:L12"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="L9:L10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4401,7 +4401,7 @@
       <c r="J4" s="1">
         <v>1530.84</v>
       </c>
-      <c r="L4" s="46"/>
+      <c r="L4" s="42"/>
       <c r="M4" s="10"/>
     </row>
     <row r="5" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4468,7 +4468,7 @@
         <v>1541.3</v>
       </c>
       <c r="L6" s="40"/>
-      <c r="N6" s="42" t="s">
+      <c r="N6" s="44" t="s">
         <v>124</v>
       </c>
     </row>
@@ -4501,7 +4501,7 @@
       <c r="J7">
         <v>1631.78</v>
       </c>
-      <c r="N7" s="47"/>
+      <c r="N7" s="45"/>
       <c r="O7" s="10"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -4580,7 +4580,7 @@
       <c r="J10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="L10" s="45"/>
+      <c r="L10" s="46"/>
       <c r="M10" s="10"/>
       <c r="N10" s="14"/>
       <c r="P10" s="14"/>
@@ -4691,7 +4691,7 @@
       <c r="J13" s="1">
         <v>1566.5</v>
       </c>
-      <c r="P13" s="44"/>
+      <c r="P13" s="47"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -4725,7 +4725,7 @@
       <c r="J14" s="1">
         <v>1453.92</v>
       </c>
-      <c r="P14" s="42" t="s">
+      <c r="P14" s="44" t="s">
         <v>122</v>
       </c>
     </row>
@@ -4761,7 +4761,7 @@
       <c r="L15" s="39" t="s">
         <v>135</v>
       </c>
-      <c r="P15" s="42"/>
+      <c r="P15" s="44"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B16">
@@ -4792,7 +4792,7 @@
       <c r="J16">
         <v>1656.98</v>
       </c>
-      <c r="L16" s="46"/>
+      <c r="L16" s="42"/>
       <c r="M16" s="10"/>
       <c r="P16" s="14"/>
     </row>
@@ -4813,12 +4813,12 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H19" s="4"/>
-      <c r="N19" s="44"/>
+      <c r="N19" s="47"/>
       <c r="O19" s="10"/>
       <c r="P19" s="14"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="N20" s="42" t="s">
+      <c r="N20" s="44" t="s">
         <v>96</v>
       </c>
     </row>
@@ -4835,7 +4835,7 @@
       <c r="L21" s="39" t="s">
         <v>96</v>
       </c>
-      <c r="N21" s="42"/>
+      <c r="N21" s="44"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -4850,7 +4850,7 @@
       <c r="F22" s="16">
         <v>100</v>
       </c>
-      <c r="L22" s="46"/>
+      <c r="L22" s="42"/>
       <c r="M22" s="10"/>
       <c r="N22" s="14"/>
     </row>
@@ -4913,7 +4913,7 @@
       <c r="A27" t="s">
         <v>83</v>
       </c>
-      <c r="P27" s="45"/>
+      <c r="P27" s="46"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -4939,11 +4939,6 @@
     <sortCondition descending="1" ref="H11:H16"/>
   </sortState>
   <mergeCells count="16">
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="L9:L10"/>
     <mergeCell ref="L23:L24"/>
     <mergeCell ref="P26:P27"/>
     <mergeCell ref="P28:P29"/>
@@ -4955,6 +4950,11 @@
     <mergeCell ref="N20:N21"/>
     <mergeCell ref="L21:L22"/>
     <mergeCell ref="L11:L12"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="L9:L10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5096,7 +5096,7 @@
       <c r="J4" s="1">
         <v>1652.44</v>
       </c>
-      <c r="L4" s="46"/>
+      <c r="L4" s="42"/>
       <c r="M4" s="10"/>
     </row>
     <row r="5" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5199,7 +5199,7 @@
       <c r="J7">
         <v>1567.06</v>
       </c>
-      <c r="N7" s="44"/>
+      <c r="N7" s="47"/>
       <c r="O7" s="10"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -5232,7 +5232,7 @@
       <c r="J8" s="10">
         <v>1467.82</v>
       </c>
-      <c r="N8" s="42" t="s">
+      <c r="N8" s="44" t="s">
         <v>142</v>
       </c>
       <c r="P8" s="14"/>
@@ -5244,7 +5244,7 @@
       <c r="L9" s="38" t="s">
         <v>143</v>
       </c>
-      <c r="N9" s="42"/>
+      <c r="N9" s="44"/>
       <c r="P9" s="14"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -5278,7 +5278,7 @@
       <c r="J10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="L10" s="45"/>
+      <c r="L10" s="46"/>
       <c r="M10" s="10"/>
       <c r="N10" s="14"/>
       <c r="P10" s="14"/>
@@ -5353,7 +5353,7 @@
         <v>1574.5</v>
       </c>
       <c r="L12" s="39"/>
-      <c r="P12" s="42" t="s">
+      <c r="P12" s="44" t="s">
         <v>136</v>
       </c>
     </row>
@@ -5389,7 +5389,7 @@
       <c r="J13" s="1">
         <v>1644.76</v>
       </c>
-      <c r="P13" s="47"/>
+      <c r="P13" s="45"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B14">
@@ -5487,7 +5487,7 @@
       <c r="J16">
         <v>1319.8</v>
       </c>
-      <c r="L16" s="46"/>
+      <c r="L16" s="42"/>
       <c r="M16" s="10"/>
       <c r="P16" s="14"/>
     </row>
@@ -5508,12 +5508,12 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H19" s="4"/>
-      <c r="N19" s="44"/>
+      <c r="N19" s="47"/>
       <c r="O19" s="10"/>
       <c r="P19" s="14"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="N20" s="42" t="s">
+      <c r="N20" s="44" t="s">
         <v>115</v>
       </c>
     </row>
@@ -5530,7 +5530,7 @@
       <c r="L21" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="N21" s="42"/>
+      <c r="N21" s="44"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
@@ -5545,7 +5545,7 @@
       <c r="F22" s="16">
         <v>100</v>
       </c>
-      <c r="L22" s="46"/>
+      <c r="L22" s="42"/>
       <c r="M22" s="10"/>
       <c r="N22" s="14"/>
     </row>
@@ -5613,7 +5613,7 @@
         <v>83</v>
       </c>
       <c r="B27" s="5"/>
-      <c r="P27" s="45"/>
+      <c r="P27" s="46"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
@@ -5642,11 +5642,6 @@
     <sortCondition descending="1" ref="H11:H16"/>
   </sortState>
   <mergeCells count="16">
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="L9:L10"/>
     <mergeCell ref="L23:L24"/>
     <mergeCell ref="P26:P27"/>
     <mergeCell ref="P28:P29"/>
@@ -5658,6 +5653,11 @@
     <mergeCell ref="N20:N21"/>
     <mergeCell ref="L21:L22"/>
     <mergeCell ref="L11:L12"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="L9:L10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5814,7 +5814,7 @@
       <c r="I4" s="1">
         <v>1957.51</v>
       </c>
-      <c r="K4" s="46"/>
+      <c r="K4" s="42"/>
       <c r="L4" s="10"/>
     </row>
     <row r="5" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5881,7 +5881,7 @@
         <v>1810.54</v>
       </c>
       <c r="K6" s="40"/>
-      <c r="M6" s="42" t="s">
+      <c r="M6" s="44" t="s">
         <v>147</v>
       </c>
     </row>
@@ -5914,7 +5914,7 @@
       <c r="I7" s="1">
         <v>1739.8</v>
       </c>
-      <c r="M7" s="47"/>
+      <c r="M7" s="45"/>
       <c r="N7" s="10"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -6006,7 +6006,7 @@
       <c r="I10">
         <v>1479.68</v>
       </c>
-      <c r="K10" s="46"/>
+      <c r="K10" s="42"/>
       <c r="L10" s="10"/>
       <c r="M10" s="14"/>
       <c r="O10" s="14"/>
@@ -6099,11 +6099,11 @@
       <c r="I13">
         <v>1391.5</v>
       </c>
-      <c r="O13" s="44"/>
+      <c r="O13" s="47"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H14" s="4"/>
-      <c r="O14" s="42" t="s">
+      <c r="O14" s="44" t="s">
         <v>145</v>
       </c>
     </row>
@@ -6112,11 +6112,11 @@
       <c r="K15" s="39" t="s">
         <v>145</v>
       </c>
-      <c r="O15" s="42"/>
+      <c r="O15" s="44"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H16" s="4"/>
-      <c r="K16" s="46"/>
+      <c r="K16" s="42"/>
       <c r="L16" s="10"/>
       <c r="O16" s="14"/>
     </row>
@@ -6137,7 +6137,7 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H19" s="4"/>
-      <c r="M19" s="44"/>
+      <c r="M19" s="47"/>
       <c r="N19" s="10"/>
       <c r="O19" s="14"/>
     </row>
@@ -6159,7 +6159,7 @@
       <c r="K21" s="39" t="s">
         <v>154</v>
       </c>
-      <c r="M21" s="42"/>
+      <c r="M21" s="44"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
@@ -6174,7 +6174,7 @@
       <c r="F22" s="16">
         <v>100</v>
       </c>
-      <c r="K22" s="46"/>
+      <c r="K22" s="42"/>
       <c r="L22" s="10"/>
       <c r="M22" s="14"/>
     </row>
@@ -6242,7 +6242,7 @@
         <v>83</v>
       </c>
       <c r="B27" s="5"/>
-      <c r="O27" s="45"/>
+      <c r="O27" s="46"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
@@ -6271,11 +6271,6 @@
     <sortCondition descending="1" ref="H2:H13"/>
   </sortState>
   <mergeCells count="16">
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="K9:K10"/>
     <mergeCell ref="K23:K24"/>
     <mergeCell ref="O26:O27"/>
     <mergeCell ref="O28:O29"/>
@@ -6287,6 +6282,11 @@
     <mergeCell ref="M20:M21"/>
     <mergeCell ref="K21:K22"/>
     <mergeCell ref="K11:K12"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="K9:K10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6443,7 +6443,7 @@
       <c r="I4" s="1">
         <v>1799.34</v>
       </c>
-      <c r="K4" s="46"/>
+      <c r="K4" s="42"/>
       <c r="L4" s="10"/>
     </row>
     <row r="5" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6510,7 +6510,7 @@
         <v>1688.86</v>
       </c>
       <c r="K6" s="40"/>
-      <c r="M6" s="42" t="s">
+      <c r="M6" s="44" t="s">
         <v>152</v>
       </c>
     </row>
@@ -6543,7 +6543,7 @@
       <c r="I7" s="1">
         <v>1626.76</v>
       </c>
-      <c r="M7" s="47"/>
+      <c r="M7" s="45"/>
       <c r="N7" s="10"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -6635,7 +6635,7 @@
       <c r="I10">
         <v>1463.02</v>
       </c>
-      <c r="K10" s="46"/>
+      <c r="K10" s="42"/>
       <c r="L10" s="10"/>
       <c r="M10" s="14"/>
       <c r="O10" s="14"/>
@@ -6728,11 +6728,11 @@
       <c r="I13">
         <v>1620.5</v>
       </c>
-      <c r="O13" s="44"/>
+      <c r="O13" s="47"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H14" s="4"/>
-      <c r="O14" s="42" t="s">
+      <c r="O14" s="44" t="s">
         <v>151</v>
       </c>
     </row>
@@ -6741,11 +6741,11 @@
       <c r="K15" s="38" t="s">
         <v>145</v>
       </c>
-      <c r="O15" s="42"/>
+      <c r="O15" s="44"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H16" s="4"/>
-      <c r="K16" s="45"/>
+      <c r="K16" s="46"/>
       <c r="L16" s="10"/>
       <c r="O16" s="14"/>
     </row>
@@ -6759,14 +6759,14 @@
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H18" s="4"/>
       <c r="K18" s="39"/>
-      <c r="M18" s="42" t="s">
+      <c r="M18" s="44" t="s">
         <v>60</v>
       </c>
       <c r="O18" s="14"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H19" s="4"/>
-      <c r="M19" s="47"/>
+      <c r="M19" s="45"/>
       <c r="N19" s="10"/>
       <c r="O19" s="14"/>
     </row>
@@ -6803,7 +6803,7 @@
       <c r="F22" s="16">
         <v>100</v>
       </c>
-      <c r="K22" s="46"/>
+      <c r="K22" s="42"/>
       <c r="L22" s="10"/>
       <c r="M22" s="14"/>
     </row>
@@ -6871,7 +6871,7 @@
         <v>83</v>
       </c>
       <c r="B27" s="5"/>
-      <c r="O27" s="46"/>
+      <c r="O27" s="42"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
@@ -6903,11 +6903,6 @@
     <sortCondition descending="1" ref="H2:H13"/>
   </sortState>
   <mergeCells count="16">
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="K9:K10"/>
     <mergeCell ref="K23:K24"/>
     <mergeCell ref="O26:O27"/>
     <mergeCell ref="O28:O29"/>
@@ -6919,6 +6914,11 @@
     <mergeCell ref="M20:M21"/>
     <mergeCell ref="K21:K22"/>
     <mergeCell ref="K11:K12"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="K9:K10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7075,7 +7075,7 @@
       <c r="I4" s="1">
         <v>1689.34</v>
       </c>
-      <c r="K4" s="46"/>
+      <c r="K4" s="42"/>
       <c r="L4" s="10"/>
     </row>
     <row r="5" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7175,7 +7175,7 @@
       <c r="I7" s="1">
         <v>1633.82</v>
       </c>
-      <c r="M7" s="44"/>
+      <c r="M7" s="47"/>
       <c r="N7" s="10"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -7204,7 +7204,7 @@
       <c r="I8">
         <v>1591.5</v>
       </c>
-      <c r="M8" s="42" t="s">
+      <c r="M8" s="44" t="s">
         <v>147</v>
       </c>
       <c r="O8" s="14"/>
@@ -7238,7 +7238,7 @@
       <c r="K9" s="38" t="s">
         <v>156</v>
       </c>
-      <c r="M9" s="42"/>
+      <c r="M9" s="44"/>
       <c r="O9" s="14"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -7267,7 +7267,7 @@
       <c r="I10">
         <v>1757.42</v>
       </c>
-      <c r="K10" s="45"/>
+      <c r="K10" s="46"/>
       <c r="L10" s="10"/>
       <c r="M10" s="14"/>
       <c r="O10" s="14"/>
@@ -7330,7 +7330,7 @@
         <v>1435.98</v>
       </c>
       <c r="K12" s="39"/>
-      <c r="O12" s="42" t="s">
+      <c r="O12" s="44" t="s">
         <v>155</v>
       </c>
     </row>
@@ -7360,7 +7360,7 @@
       <c r="I13">
         <v>1443.12</v>
       </c>
-      <c r="O13" s="47"/>
+      <c r="O13" s="45"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H14" s="4"/>
@@ -7377,7 +7377,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H16" s="4"/>
-      <c r="K16" s="46"/>
+      <c r="K16" s="42"/>
       <c r="L16" s="10"/>
       <c r="O16" s="14"/>
     </row>
@@ -7391,14 +7391,14 @@
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H18" s="4"/>
       <c r="K18" s="38"/>
-      <c r="M18" s="42" t="s">
+      <c r="M18" s="44" t="s">
         <v>145</v>
       </c>
       <c r="O18" s="14"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H19" s="4"/>
-      <c r="M19" s="47"/>
+      <c r="M19" s="45"/>
       <c r="N19" s="10"/>
       <c r="O19" s="14"/>
     </row>
@@ -7435,7 +7435,7 @@
       <c r="F22" s="16">
         <v>100</v>
       </c>
-      <c r="K22" s="46"/>
+      <c r="K22" s="42"/>
       <c r="L22" s="10"/>
       <c r="M22" s="14"/>
     </row>
@@ -7503,7 +7503,7 @@
         <v>83</v>
       </c>
       <c r="B27" s="5"/>
-      <c r="O27" s="46"/>
+      <c r="O27" s="42"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
@@ -7535,11 +7535,6 @@
     <sortCondition descending="1" ref="H2:H13"/>
   </sortState>
   <mergeCells count="16">
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="K9:K10"/>
     <mergeCell ref="K23:K24"/>
     <mergeCell ref="O26:O27"/>
     <mergeCell ref="O28:O29"/>
@@ -7551,6 +7546,11 @@
     <mergeCell ref="M20:M21"/>
     <mergeCell ref="K21:K22"/>
     <mergeCell ref="K11:K12"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="K9:K10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7560,8 +7560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DC38AAB-96CB-42DE-9F89-BEE07C09AAC6}">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O30" sqref="O30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7607,7 +7607,9 @@
       </c>
     </row>
     <row r="2" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
@@ -7644,7 +7646,9 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
       <c r="B3" s="1">
         <v>2</v>
       </c>
@@ -7675,7 +7679,9 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
       <c r="B4" s="1">
         <v>3</v>
       </c>
@@ -7701,11 +7707,13 @@
       <c r="I4" s="1">
         <v>1781.88</v>
       </c>
-      <c r="K4" s="46"/>
+      <c r="K4" s="42"/>
       <c r="L4" s="10"/>
     </row>
     <row r="5" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
       <c r="B5" s="1">
         <v>4</v>
       </c>
@@ -7737,7 +7745,9 @@
       <c r="M5" s="14"/>
     </row>
     <row r="6" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
       <c r="B6" s="1">
         <v>5</v>
       </c>
@@ -7769,7 +7779,9 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
       <c r="B7" s="1">
         <v>6</v>
       </c>
@@ -7795,10 +7807,13 @@
       <c r="I7" s="1">
         <v>1821.42</v>
       </c>
-      <c r="M7" s="44"/>
+      <c r="M7" s="47"/>
       <c r="N7" s="10"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
       <c r="B8">
         <v>7</v>
       </c>
@@ -7824,12 +7839,15 @@
       <c r="I8">
         <v>1771.9</v>
       </c>
-      <c r="M8" s="42" t="s">
+      <c r="M8" s="44" t="s">
         <v>276</v>
       </c>
       <c r="O8" s="14"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
       <c r="B9">
         <v>8</v>
       </c>
@@ -7858,10 +7876,13 @@
       <c r="K9" s="39" t="s">
         <v>276</v>
       </c>
-      <c r="M9" s="42"/>
+      <c r="M9" s="44"/>
       <c r="O9" s="14"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
       <c r="B10">
         <v>9</v>
       </c>
@@ -7887,12 +7908,15 @@
       <c r="I10">
         <v>1709.36</v>
       </c>
-      <c r="K10" s="46"/>
+      <c r="K10" s="42"/>
       <c r="L10" s="10"/>
       <c r="M10" s="14"/>
       <c r="O10" s="14"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
       <c r="B11">
         <v>10</v>
       </c>
@@ -7953,7 +7977,7 @@
         <v>1418.44</v>
       </c>
       <c r="K12" s="38"/>
-      <c r="O12" s="42" t="s">
+      <c r="O12" s="43" t="s">
         <v>147</v>
       </c>
     </row>
@@ -7999,11 +8023,11 @@
       <c r="K15" s="39" t="s">
         <v>145</v>
       </c>
-      <c r="O15" s="42"/>
+      <c r="O15" s="44"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H16" s="4"/>
-      <c r="K16" s="46"/>
+      <c r="K16" s="42"/>
       <c r="L16" s="10"/>
       <c r="O16" s="14"/>
     </row>
@@ -8017,14 +8041,14 @@
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H18" s="4"/>
       <c r="K18" s="38"/>
-      <c r="M18" s="42" t="s">
+      <c r="M18" s="44" t="s">
         <v>145</v>
       </c>
       <c r="O18" s="14"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H19" s="4"/>
-      <c r="M19" s="47"/>
+      <c r="M19" s="45"/>
       <c r="N19" s="10"/>
       <c r="O19" s="14"/>
     </row>
@@ -8061,7 +8085,7 @@
       <c r="F22" s="16">
         <v>100</v>
       </c>
-      <c r="K22" s="46"/>
+      <c r="K22" s="42"/>
       <c r="L22" s="10"/>
       <c r="M22" s="14"/>
     </row>
@@ -8120,7 +8144,7 @@
       <c r="F26" s="16">
         <v>10</v>
       </c>
-      <c r="O26" s="38" t="s">
+      <c r="O26" s="39" t="s">
         <v>145</v>
       </c>
     </row>
@@ -8129,7 +8153,7 @@
         <v>83</v>
       </c>
       <c r="B27" s="5"/>
-      <c r="O27" s="45"/>
+      <c r="O27" s="42"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
@@ -8158,11 +8182,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="K9:K10"/>
     <mergeCell ref="K23:K24"/>
     <mergeCell ref="O26:O27"/>
     <mergeCell ref="O28:O29"/>
@@ -8174,6 +8193,11 @@
     <mergeCell ref="M20:M21"/>
     <mergeCell ref="K21:K22"/>
     <mergeCell ref="K11:K12"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="K9:K10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8184,8 +8208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5B52E80-2A72-48E8-8AE2-03BD1ED3BA86}">
   <dimension ref="A1:AU81"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AW7" sqref="AW7"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="X28" sqref="X28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8486,11 +8510,11 @@
       </c>
       <c r="AP2" s="32">
         <f>_xlfn.XLOOKUP($A2,'2024'!$D$2:$D$13,'2024'!$A$2:$A$13,"x")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AQ2" s="4">
         <f>COUNTIF(AC2:AP2,"&gt;0")/COUNTIF(AC2:AO2,"&lt;&gt;x")</f>
-        <v>0.46153846153846156</v>
+        <v>0.53846153846153844</v>
       </c>
       <c r="AR2">
         <f>COUNTIF($AC2:$AP2,AR$1)</f>
@@ -8502,11 +8526,11 @@
       </c>
       <c r="AT2">
         <f>COUNTIF($AC2:$AP2,AT$1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AU2" s="4">
         <f>(AT2+(AS2*2)+(AR2*3))/COUNTIF(AC2:AP2,"&lt;&gt;x")</f>
-        <v>0.42857142857142855</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:47" x14ac:dyDescent="0.25">
@@ -9174,11 +9198,11 @@
       </c>
       <c r="AP6" s="32">
         <f>_xlfn.XLOOKUP($A6,'2024'!$D$2:$D$13,'2024'!$A$2:$A$13,"x")</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AQ6" s="4">
         <f t="shared" si="0"/>
-        <v>0.53846153846153844</v>
+        <v>0.61538461538461542</v>
       </c>
       <c r="AR6">
         <f t="shared" si="1"/>
@@ -9690,15 +9714,15 @@
       </c>
       <c r="AP9" s="32">
         <f>_xlfn.XLOOKUP($A9,'2024'!$D$2:$D$13,'2024'!$A$2:$A$13,"x")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ9" s="4">
         <f t="shared" si="0"/>
-        <v>0.46153846153846156</v>
+        <v>0.53846153846153844</v>
       </c>
       <c r="AR9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS9">
         <f t="shared" si="1"/>
@@ -9710,7 +9734,7 @@
       </c>
       <c r="AU9" s="4">
         <f t="shared" si="2"/>
-        <v>0.14285714285714285</v>
+        <v>0.35714285714285715</v>
       </c>
     </row>
     <row r="10" spans="1:47" x14ac:dyDescent="0.25">
@@ -10034,11 +10058,11 @@
       </c>
       <c r="AP11" s="32">
         <f>_xlfn.XLOOKUP($A11,'2024'!$D$2:$D$13,'2024'!$A$2:$A$13,"x")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AQ11" s="4">
         <f t="shared" si="0"/>
-        <v>0.66666666666666663</v>
+        <v>0.75</v>
       </c>
       <c r="AR11">
         <f t="shared" si="1"/>
@@ -10046,7 +10070,7 @@
       </c>
       <c r="AS11">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AT11">
         <f t="shared" si="1"/>
@@ -10054,7 +10078,7 @@
       </c>
       <c r="AU11" s="4">
         <f t="shared" si="2"/>
-        <v>1.0769230769230769</v>
+        <v>1.2307692307692308</v>
       </c>
     </row>
     <row r="12" spans="1:47" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -10378,11 +10402,11 @@
       </c>
       <c r="AP13" s="32">
         <f>_xlfn.XLOOKUP($A13,'2024'!$D$2:$D$13,'2024'!$A$2:$A$13,"x")</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AQ13" s="4">
         <f t="shared" si="0"/>
-        <v>0.25</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="AR13">
         <f t="shared" si="1"/>
@@ -10550,11 +10574,11 @@
       </c>
       <c r="AP14" s="32">
         <f>_xlfn.XLOOKUP($A14,'2024'!$D$2:$D$13,'2024'!$A$2:$A$13,"x")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AQ14" s="4">
         <f t="shared" si="0"/>
-        <v>0.54545454545454541</v>
+        <v>0.63636363636363635</v>
       </c>
       <c r="AR14">
         <f t="shared" si="1"/>
@@ -11238,11 +11262,11 @@
       </c>
       <c r="AP18" s="32">
         <f>_xlfn.XLOOKUP($A18,'2024'!$D$2:$D$13,'2024'!$A$2:$A$13,"x")</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="AQ18" s="4">
         <f t="shared" si="0"/>
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="AR18">
         <f t="shared" si="1"/>
@@ -11410,11 +11434,11 @@
       </c>
       <c r="AP19" s="32">
         <f>_xlfn.XLOOKUP($A19,'2024'!$D$2:$D$13,'2024'!$A$2:$A$13,"x")</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AQ19" s="4">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="AR19">
         <f t="shared" si="1"/>
@@ -12098,11 +12122,11 @@
       </c>
       <c r="AP23" s="32">
         <f>_xlfn.XLOOKUP($A23,'2024'!$D$2:$D$13,'2024'!$A$2:$A$13,"x")</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AQ23" s="4">
         <f t="shared" si="0"/>
-        <v>0.42857142857142855</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="AR23">
         <f t="shared" si="1"/>
@@ -12442,11 +12466,11 @@
       </c>
       <c r="AP25" s="32">
         <f>_xlfn.XLOOKUP($A25,'2024'!$D$2:$D$13,'2024'!$A$2:$A$13,"x")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AQ25" s="4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AR25">
         <f t="shared" si="1"/>
@@ -18251,7 +18275,7 @@
       <c r="J4" s="1">
         <v>1481.24</v>
       </c>
-      <c r="L4" s="46"/>
+      <c r="L4" s="42"/>
       <c r="M4" s="10"/>
     </row>
     <row r="5" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -18324,7 +18348,7 @@
         <v>1635.62</v>
       </c>
       <c r="L6" s="40"/>
-      <c r="N6" s="42" t="s">
+      <c r="N6" s="44" t="s">
         <v>79</v>
       </c>
     </row>
@@ -18357,7 +18381,7 @@
       <c r="J7">
         <v>1508.98</v>
       </c>
-      <c r="N7" s="47"/>
+      <c r="N7" s="45"/>
       <c r="O7" s="10"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -18436,7 +18460,7 @@
       <c r="J10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="L10" s="46"/>
+      <c r="L10" s="42"/>
       <c r="M10" s="10"/>
       <c r="N10" s="14"/>
       <c r="P10" s="14"/>
@@ -18544,7 +18568,7 @@
       <c r="J13">
         <v>1539.26</v>
       </c>
-      <c r="P13" s="44"/>
+      <c r="P13" s="47"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B14">
@@ -18575,7 +18599,7 @@
       <c r="J14">
         <v>1336.24</v>
       </c>
-      <c r="P14" s="42" t="s">
+      <c r="P14" s="44" t="s">
         <v>70</v>
       </c>
     </row>
@@ -18611,7 +18635,7 @@
       <c r="L15" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="P15" s="42"/>
+      <c r="P15" s="44"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B16">
@@ -18642,7 +18666,7 @@
       <c r="J16">
         <v>1513.46</v>
       </c>
-      <c r="L16" s="45"/>
+      <c r="L16" s="46"/>
       <c r="M16" s="10"/>
       <c r="P16" s="14"/>
     </row>
@@ -18656,14 +18680,14 @@
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H18" s="4"/>
       <c r="L18" s="39"/>
-      <c r="N18" s="42" t="s">
+      <c r="N18" s="44" t="s">
         <v>70</v>
       </c>
       <c r="P18" s="14"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H19" s="4"/>
-      <c r="N19" s="47"/>
+      <c r="N19" s="45"/>
       <c r="O19" s="10"/>
       <c r="P19" s="14"/>
     </row>
@@ -18700,7 +18724,7 @@
       <c r="F22" s="16">
         <v>60</v>
       </c>
-      <c r="L22" s="46"/>
+      <c r="L22" s="42"/>
       <c r="M22" s="10"/>
       <c r="N22" s="14"/>
     </row>
@@ -18744,7 +18768,7 @@
       <c r="A27" t="s">
         <v>83</v>
       </c>
-      <c r="P27" s="45"/>
+      <c r="P27" s="46"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -18765,6 +18789,12 @@
     <sortCondition descending="1" ref="H11:H16"/>
   </sortState>
   <mergeCells count="16">
+    <mergeCell ref="P14:P15"/>
+    <mergeCell ref="P12:P13"/>
+    <mergeCell ref="P28:P29"/>
+    <mergeCell ref="P26:P27"/>
+    <mergeCell ref="L23:L24"/>
+    <mergeCell ref="L21:L22"/>
     <mergeCell ref="L3:L4"/>
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="N8:N9"/>
@@ -18775,12 +18805,6 @@
     <mergeCell ref="L11:L12"/>
     <mergeCell ref="L15:L16"/>
     <mergeCell ref="L17:L18"/>
-    <mergeCell ref="P14:P15"/>
-    <mergeCell ref="P12:P13"/>
-    <mergeCell ref="P28:P29"/>
-    <mergeCell ref="P26:P27"/>
-    <mergeCell ref="L23:L24"/>
-    <mergeCell ref="L21:L22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18922,7 +18946,7 @@
       <c r="J4" s="1">
         <v>1639.06</v>
       </c>
-      <c r="L4" s="46"/>
+      <c r="L4" s="42"/>
       <c r="M4" s="10"/>
     </row>
     <row r="5" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -18995,7 +19019,7 @@
         <v>1643.26</v>
       </c>
       <c r="L6" s="40"/>
-      <c r="N6" s="42" t="s">
+      <c r="N6" s="44" t="s">
         <v>86</v>
       </c>
     </row>
@@ -19028,7 +19052,7 @@
       <c r="J7">
         <v>1588.24</v>
       </c>
-      <c r="N7" s="47"/>
+      <c r="N7" s="45"/>
       <c r="O7" s="10"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -19107,7 +19131,7 @@
       <c r="J10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="L10" s="45"/>
+      <c r="L10" s="46"/>
       <c r="M10" s="10"/>
       <c r="N10" s="14"/>
       <c r="P10" s="14"/>
@@ -19215,7 +19239,7 @@
       <c r="J13">
         <v>1497.04</v>
       </c>
-      <c r="P13" s="44"/>
+      <c r="P13" s="47"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B14">
@@ -19246,7 +19270,7 @@
       <c r="J14">
         <v>1303.76</v>
       </c>
-      <c r="P14" s="42" t="s">
+      <c r="P14" s="44" t="s">
         <v>88</v>
       </c>
     </row>
@@ -19282,7 +19306,7 @@
       <c r="L15" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="P15" s="42"/>
+      <c r="P15" s="44"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B16">
@@ -19313,7 +19337,7 @@
       <c r="J16">
         <v>1382.22</v>
       </c>
-      <c r="L16" s="45"/>
+      <c r="L16" s="46"/>
       <c r="M16" s="10"/>
       <c r="P16" s="14"/>
     </row>
@@ -19327,14 +19351,14 @@
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H18" s="4"/>
       <c r="L18" s="39"/>
-      <c r="N18" s="42" t="s">
+      <c r="N18" s="44" t="s">
         <v>72</v>
       </c>
       <c r="P18" s="14"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H19" s="4"/>
-      <c r="N19" s="47"/>
+      <c r="N19" s="45"/>
       <c r="O19" s="10"/>
       <c r="P19" s="14"/>
     </row>
@@ -19371,7 +19395,7 @@
       <c r="F22" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="L22" s="46"/>
+      <c r="L22" s="42"/>
       <c r="M22" s="10"/>
       <c r="N22" s="14"/>
     </row>
@@ -19420,7 +19444,7 @@
       <c r="A27" t="s">
         <v>83</v>
       </c>
-      <c r="P27" s="46"/>
+      <c r="P27" s="42"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -19441,11 +19465,6 @@
     <sortCondition descending="1" ref="H11:H16"/>
   </sortState>
   <mergeCells count="16">
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="L9:L10"/>
     <mergeCell ref="L23:L24"/>
     <mergeCell ref="P26:P27"/>
     <mergeCell ref="P28:P29"/>
@@ -19457,6 +19476,11 @@
     <mergeCell ref="N20:N21"/>
     <mergeCell ref="L21:L22"/>
     <mergeCell ref="L11:L12"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="L9:L10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>